<commit_message>
podcast description spacing adjustment
</commit_message>
<xml_diff>
--- a/data/calendar.xlsx
+++ b/data/calendar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="480">
   <si>
     <t>key</t>
   </si>
@@ -32,7 +32,7 @@
   </si>
   <si>
     <t>1.&amp;nbsp;Delegate numbers shown are the total number available for a given state. Each state and party has its own rules for awarding delegates to candidates. Some state parties award delegates proportionally depending on the results of a caucus, primary or party convention. Other party primaries and caucuses are winner-take-all. Still others are hybrids.&lt;br /&gt;
-2.&amp;nbsp;On the Republican side, American Samoa, Colorado, Guam, North Dakota and Wyoming will not select delegates via caucuses or primaries. In &lt;a href="http://www.thegreenpapers.com/P16/WY-R"&gt;Wyoming&lt;/a&gt;, delegates will be selected at county conventions beginning on March 12.&lt;br /&gt;
+2.&amp;nbsp;On the Republican side, American Samoa, Colorado, Guam, North Dakota, the U.S. Virgin Islands and Wyoming will not select delegates via caucuses or primaries. In &lt;a href="http://www.thegreenpapers.com/P16/WY-R"&gt;Wyoming&lt;/a&gt;, delegates will be selected at county conventions beginning on March 12.&lt;br /&gt;
 3.&amp;nbsp;On the Democratic side, delegate figures include both delegates awarded via the primary/caucus process and "&lt;a href="http://www.npr.org/2015/11/13/455812702/clinton-has-45-to-1-superdelegate-advantage-over-sanders"&gt;superdelegates,&lt;/a&gt;" who may vote as they wish.&lt;br /&gt;
 4.&amp;nbsp;Nebraska will hold presidential primaries on May 10. However, the Democratic Party will use a separate caucus on March 5 to determine its delegate allocation.&lt;br /&gt;
 5.&amp;nbsp;Washington will hold presidential primaries on May 24. However, the Democratic Party will use will use a separate caucus on March 26 to determine its delegate allocation.&lt;br /&gt;
@@ -2536,7 +2536,9 @@
       <c r="I11" s="19"/>
       <c r="J11" s="20"/>
       <c r="K11" s="21"/>
-      <c r="L11" s="35"/>
+      <c r="L11" s="22" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="23" t="s">
@@ -2566,7 +2568,9 @@
       <c r="K12" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="L12" s="35"/>
+      <c r="L12" s="22" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="15" t="s">
@@ -16970,7 +16974,27 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="70"/>
+      <c r="A7" s="80" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="D7" s="37">
+        <v>73.5</v>
+      </c>
+      <c r="F7" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="37" t="s">
+        <v>333</v>
+      </c>
+      <c r="H7" s="37">
+        <v>26.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="70"/>

</xml_diff>

<commit_message>
don't include full poll closing for pr
</commit_message>
<xml_diff>
--- a/data/calendar.xlsx
+++ b/data/calendar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="482">
   <si>
     <t>key</t>
   </si>
@@ -513,6 +513,9 @@
   </si>
   <si>
     <t>Tuesday, March 8</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
   <si>
     <t>3/8/2016</t>
@@ -3555,6 +3558,12 @@
         <v>38</v>
       </c>
       <c r="L36" s="55"/>
+      <c r="M36" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="N36" s="49">
+        <v>42435.833333333336</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="23" t="s">
@@ -3583,6 +3592,8 @@
         <v>49</v>
       </c>
       <c r="L37" s="55"/>
+      <c r="M37" s="36"/>
+      <c r="N37" s="49"/>
     </row>
     <row r="38">
       <c r="A38" s="15" t="s">
@@ -3601,20 +3612,23 @@
       <c r="J38" s="20"/>
       <c r="K38" s="21"/>
       <c r="L38" s="55"/>
+      <c r="M38" s="36" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C39" s="31"/>
       <c r="D39" s="25" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F39" s="26"/>
       <c r="G39" s="33"/>
@@ -3623,7 +3637,7 @@
         <v>36</v>
       </c>
       <c r="J39" s="30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K39" s="23" t="s">
         <v>38</v>
@@ -3635,14 +3649,14 @@
         <v>15</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C40" s="31"/>
       <c r="D40" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F40" s="26"/>
       <c r="G40" s="46"/>
@@ -3663,21 +3677,21 @@
         <v>15</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C41" s="31"/>
       <c r="D41" s="25" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F41" s="26"/>
       <c r="G41" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H41" s="30" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I41" s="29" t="s">
         <v>47</v>
@@ -3695,21 +3709,21 @@
         <v>15</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C42" s="31"/>
       <c r="D42" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F42" s="26"/>
       <c r="G42" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I42" s="29" t="s">
         <v>47</v>
@@ -3727,7 +3741,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21"/>
@@ -3745,14 +3759,14 @@
         <v>15</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C44" s="25"/>
       <c r="D44" s="25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F44" s="26"/>
       <c r="G44" s="33"/>
@@ -3761,7 +3775,7 @@
         <v>36</v>
       </c>
       <c r="J44" s="30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K44" s="23" t="s">
         <v>38</v>
@@ -3773,7 +3787,7 @@
         <v>15</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C45" s="31"/>
       <c r="D45" s="25" t="s">
@@ -3786,13 +3800,13 @@
       <c r="G45" s="33"/>
       <c r="H45" s="34"/>
       <c r="I45" s="56" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J45" s="57" t="s">
         <v>129</v>
       </c>
       <c r="K45" s="24" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L45" s="55"/>
     </row>
@@ -3801,21 +3815,21 @@
         <v>15</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C46" s="38"/>
       <c r="D46" s="38" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E46" s="43" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F46" s="43"/>
       <c r="G46" s="39" t="s">
         <v>133</v>
       </c>
       <c r="H46" s="40" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I46" s="44"/>
       <c r="J46" s="45"/>
@@ -3829,7 +3843,7 @@
         <v>27</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="17"/>
@@ -3847,27 +3861,27 @@
         <v>15</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C48" s="31"/>
       <c r="D48" s="25" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F48" s="26"/>
       <c r="G48" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I48" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J48" s="30" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K48" s="23" t="s">
         <v>49</v>
@@ -3879,27 +3893,27 @@
         <v>15</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C49" s="31"/>
       <c r="D49" s="25" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F49" s="26"/>
       <c r="G49" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I49" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J49" s="30" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="K49" s="23" t="s">
         <v>49</v>
@@ -3911,21 +3925,21 @@
         <v>15</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="25" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F50" s="26"/>
       <c r="G50" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I50" s="29" t="s">
         <v>47</v>
@@ -3943,27 +3957,27 @@
         <v>15</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C51" s="31"/>
       <c r="D51" s="25" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F51" s="26"/>
       <c r="G51" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H51" s="30" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I51" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J51" s="30" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K51" s="23" t="s">
         <v>49</v>
@@ -3975,27 +3989,27 @@
         <v>15</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C52" s="31"/>
       <c r="D52" s="25" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F52" s="26"/>
       <c r="G52" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H52" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I52" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J52" s="30" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K52" s="23" t="s">
         <v>49</v>
@@ -4007,23 +4021,23 @@
         <v>15</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C53" s="38"/>
       <c r="D53" s="38" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E53" s="43" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F53" s="43"/>
       <c r="G53" s="44"/>
       <c r="H53" s="45"/>
       <c r="I53" s="39" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J53" s="40" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K53" s="41" t="s">
         <v>38</v>
@@ -4035,7 +4049,7 @@
         <v>27</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="21"/>
@@ -4053,23 +4067,23 @@
         <v>15</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C55" s="38"/>
       <c r="D55" s="38" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E55" s="43" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F55" s="43"/>
       <c r="G55" s="44"/>
       <c r="H55" s="45"/>
       <c r="I55" s="39" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J55" s="40" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K55" s="41" t="s">
         <v>38</v>
@@ -4081,7 +4095,7 @@
         <v>27</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C56" s="21"/>
       <c r="D56" s="21"/>
@@ -4099,21 +4113,21 @@
         <v>15</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C57" s="31"/>
       <c r="D57" s="25" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E57" s="26" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F57" s="26"/>
       <c r="G57" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H57" s="30" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I57" s="29" t="s">
         <v>47</v>
@@ -4131,21 +4145,21 @@
         <v>15</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C58" s="25"/>
       <c r="D58" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E58" s="26" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F58" s="26"/>
       <c r="G58" s="29" t="s">
         <v>34</v>
       </c>
       <c r="H58" s="30" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I58" s="33"/>
       <c r="J58" s="34"/>
@@ -4159,14 +4173,14 @@
         <v>15</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C59" s="25"/>
       <c r="D59" s="25" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E59" s="26" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F59" s="26"/>
       <c r="G59" s="29" t="s">
@@ -4191,7 +4205,7 @@
         <v>15</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C60" s="38"/>
       <c r="D60" s="38" t="s">
@@ -4204,10 +4218,10 @@
       <c r="G60" s="44"/>
       <c r="H60" s="45"/>
       <c r="I60" s="46" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J60" s="47" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K60" s="41" t="s">
         <v>38</v>
@@ -4219,7 +4233,7 @@
         <v>27</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C61" s="58"/>
       <c r="D61" s="21"/>
@@ -4237,7 +4251,7 @@
         <v>15</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C62" s="25"/>
       <c r="D62" s="25" t="s">
@@ -4251,7 +4265,7 @@
         <v>34</v>
       </c>
       <c r="H62" s="30" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I62" s="33"/>
       <c r="J62" s="34"/>
@@ -4265,21 +4279,21 @@
         <v>15</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C63" s="25"/>
       <c r="D63" s="25" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E63" s="26" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F63" s="26"/>
       <c r="G63" s="29" t="s">
         <v>34</v>
       </c>
       <c r="H63" s="30" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="I63" s="33"/>
       <c r="J63" s="34"/>
@@ -4293,21 +4307,21 @@
         <v>15</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C64" s="31"/>
       <c r="D64" s="25" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E64" s="26" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F64" s="26"/>
       <c r="G64" s="29" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H64" s="30" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I64" s="33"/>
       <c r="J64" s="34"/>
@@ -4321,7 +4335,7 @@
         <v>27</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C65" s="21"/>
       <c r="D65" s="21"/>
@@ -4339,21 +4353,21 @@
         <v>15</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C66" s="31"/>
       <c r="D66" s="25" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E66" s="26" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F66" s="26"/>
       <c r="G66" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H66" s="30" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="I66" s="59" t="s">
         <v>47</v>
@@ -4371,7 +4385,7 @@
         <v>27</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C67" s="21"/>
       <c r="D67" s="21"/>
@@ -4389,7 +4403,7 @@
         <v>15</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C68" s="25"/>
       <c r="D68" s="25" t="s">
@@ -4403,7 +4417,7 @@
         <v>34</v>
       </c>
       <c r="H68" s="30" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I68" s="33"/>
       <c r="J68" s="34"/>
@@ -4417,7 +4431,7 @@
         <v>27</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C69" s="21"/>
       <c r="D69" s="21"/>
@@ -4435,27 +4449,27 @@
         <v>15</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C70" s="31"/>
       <c r="D70" s="25" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E70" s="26" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F70" s="26"/>
       <c r="G70" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H70" s="30" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I70" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J70" s="30" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K70" s="23" t="s">
         <v>49</v>
@@ -4467,7 +4481,7 @@
         <v>27</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C71" s="21"/>
       <c r="D71" s="21"/>
@@ -4485,21 +4499,21 @@
         <v>15</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C72" s="31"/>
       <c r="D72" s="25" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E72" s="26" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F72" s="26"/>
       <c r="G72" s="59" t="s">
         <v>45</v>
       </c>
       <c r="H72" s="60" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I72" s="29" t="s">
         <v>47</v>
@@ -4517,21 +4531,21 @@
         <v>15</v>
       </c>
       <c r="B73" s="24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C73" s="31"/>
       <c r="D73" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E73" s="26" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F73" s="26"/>
       <c r="G73" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H73" s="30" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="I73" s="29" t="s">
         <v>47</v>
@@ -4549,21 +4563,21 @@
         <v>15</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C74" s="31"/>
       <c r="D74" s="25" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E74" s="26" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F74" s="26"/>
       <c r="G74" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H74" s="30" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I74" s="29" t="s">
         <v>45</v>
@@ -4581,27 +4595,27 @@
         <v>15</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C75" s="31"/>
       <c r="D75" s="25" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E75" s="26" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F75" s="26"/>
       <c r="G75" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H75" s="30" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I75" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J75" s="30" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="K75" s="23" t="s">
         <v>49</v>
@@ -4613,27 +4627,27 @@
         <v>15</v>
       </c>
       <c r="B76" s="24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C76" s="31"/>
       <c r="D76" s="25" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E76" s="26" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F76" s="26"/>
       <c r="G76" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H76" s="30" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I76" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J76" s="30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K76" s="23" t="s">
         <v>49</v>
@@ -4645,7 +4659,7 @@
         <v>27</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C77" s="21"/>
       <c r="D77" s="21"/>
@@ -4663,27 +4677,27 @@
         <v>15</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C78" s="31"/>
       <c r="D78" s="25" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E78" s="26" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F78" s="26"/>
       <c r="G78" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H78" s="30" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I78" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J78" s="30" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K78" s="23" t="s">
         <v>49</v>
@@ -4695,7 +4709,7 @@
         <v>27</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C79" s="21"/>
       <c r="D79" s="21"/>
@@ -4713,21 +4727,21 @@
         <v>15</v>
       </c>
       <c r="B80" s="37" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C80" s="38"/>
       <c r="D80" s="38" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E80" s="43" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F80" s="43"/>
       <c r="G80" s="39" t="s">
         <v>34</v>
       </c>
       <c r="H80" s="40" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I80" s="44"/>
       <c r="J80" s="45"/>
@@ -4741,7 +4755,7 @@
         <v>27</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C81" s="21"/>
       <c r="D81" s="21"/>
@@ -4759,7 +4773,7 @@
         <v>15</v>
       </c>
       <c r="B82" s="24" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C82" s="31"/>
       <c r="D82" s="25" t="s">
@@ -4770,7 +4784,7 @@
       </c>
       <c r="F82" s="26"/>
       <c r="G82" s="56" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H82" s="57" t="s">
         <v>37</v>
@@ -4779,7 +4793,7 @@
         <v>47</v>
       </c>
       <c r="J82" s="30" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K82" s="23" t="s">
         <v>49</v>
@@ -4791,14 +4805,14 @@
         <v>15</v>
       </c>
       <c r="B83" s="24" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C83" s="31"/>
       <c r="D83" s="25" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E83" s="26" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F83" s="26"/>
       <c r="G83" s="29" t="s">
@@ -4811,7 +4825,7 @@
         <v>47</v>
       </c>
       <c r="J83" s="30" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="K83" s="23" t="s">
         <v>49</v>
@@ -4823,7 +4837,7 @@
         <v>27</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C84" s="21"/>
       <c r="D84" s="21"/>
@@ -4841,7 +4855,7 @@
         <v>15</v>
       </c>
       <c r="B85" s="24" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C85" s="31"/>
       <c r="D85" s="25" t="s">
@@ -4855,7 +4869,7 @@
         <v>45</v>
       </c>
       <c r="H85" s="30" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="I85" s="33"/>
       <c r="J85" s="34"/>
@@ -4869,21 +4883,21 @@
         <v>15</v>
       </c>
       <c r="B86" s="24" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C86" s="31"/>
       <c r="D86" s="25" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E86" s="26" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F86" s="26"/>
       <c r="G86" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H86" s="30" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I86" s="29" t="s">
         <v>47</v>
@@ -4901,7 +4915,7 @@
         <v>27</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C87" s="21"/>
       <c r="D87" s="21"/>
@@ -4919,27 +4933,27 @@
         <v>15</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C88" s="25"/>
       <c r="D88" s="25" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F88" s="26"/>
       <c r="G88" s="56" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H88" s="57" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I88" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J88" s="30" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="K88" s="23" t="s">
         <v>49</v>
@@ -4951,7 +4965,7 @@
         <v>27</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C89" s="21"/>
       <c r="D89" s="21"/>
@@ -4969,21 +4983,21 @@
         <v>15</v>
       </c>
       <c r="B90" s="37" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C90" s="48"/>
       <c r="D90" s="38" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E90" s="43" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F90" s="43"/>
       <c r="G90" s="39" t="s">
         <v>133</v>
       </c>
       <c r="H90" s="40" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I90" s="44"/>
       <c r="J90" s="45"/>
@@ -4997,7 +5011,7 @@
         <v>27</v>
       </c>
       <c r="B91" s="61" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C91" s="21"/>
       <c r="D91" s="21"/>
@@ -5015,7 +5029,7 @@
         <v>15</v>
       </c>
       <c r="B92" s="62" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C92" s="63"/>
       <c r="D92" s="64" t="s">
@@ -5029,7 +5043,7 @@
         <v>34</v>
       </c>
       <c r="H92" s="67" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="I92" s="68"/>
       <c r="J92" s="69"/>
@@ -5043,7 +5057,7 @@
         <v>27</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C93" s="21"/>
       <c r="D93" s="21"/>
@@ -5061,27 +5075,27 @@
         <v>15</v>
       </c>
       <c r="B94" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C94" s="31"/>
       <c r="D94" s="25" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E94" s="26" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F94" s="26"/>
       <c r="G94" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H94" s="30" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="I94" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J94" s="30" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="K94" s="23" t="s">
         <v>49</v>
@@ -5093,27 +5107,27 @@
         <v>15</v>
       </c>
       <c r="B95" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C95" s="31"/>
       <c r="D95" s="25" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E95" s="26" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F95" s="26"/>
       <c r="G95" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H95" s="30" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I95" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J95" s="30" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K95" s="23" t="s">
         <v>49</v>
@@ -5125,27 +5139,27 @@
         <v>15</v>
       </c>
       <c r="B96" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C96" s="31"/>
       <c r="D96" s="25" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E96" s="26" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F96" s="26"/>
       <c r="G96" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H96" s="30" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I96" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J96" s="30" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K96" s="23" t="s">
         <v>49</v>
@@ -5157,14 +5171,14 @@
         <v>15</v>
       </c>
       <c r="B97" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C97" s="31"/>
       <c r="D97" s="25" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E97" s="26" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F97" s="26"/>
       <c r="G97" s="29" t="s">
@@ -5177,7 +5191,7 @@
         <v>47</v>
       </c>
       <c r="J97" s="30" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="K97" s="23" t="s">
         <v>49</v>
@@ -5189,14 +5203,14 @@
         <v>15</v>
       </c>
       <c r="B98" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C98" s="31"/>
       <c r="D98" s="25" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E98" s="26" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F98" s="26"/>
       <c r="G98" s="29" t="s">
@@ -5217,21 +5231,21 @@
         <v>15</v>
       </c>
       <c r="B99" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C99" s="31"/>
       <c r="D99" s="25" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E99" s="26" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F99" s="26"/>
       <c r="G99" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H99" s="30" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I99" s="29" t="s">
         <v>47</v>
@@ -5249,7 +5263,7 @@
         <v>27</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C100" s="21"/>
       <c r="D100" s="21"/>
@@ -5267,21 +5281,21 @@
         <v>15</v>
       </c>
       <c r="B101" s="24" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C101" s="31"/>
       <c r="D101" s="25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E101" s="26" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F101" s="26"/>
       <c r="G101" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H101" s="30" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="I101" s="33"/>
       <c r="J101" s="34"/>
@@ -16919,46 +16933,46 @@
         <v>16</v>
       </c>
       <c r="C1" s="80" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D1" s="80" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E1" s="80" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F1" s="80" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G1" s="80" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="H1" s="80" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="I1" s="80" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J1" s="80" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="K1" s="80" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="L1" s="80" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="M1" s="80" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="N1" s="80" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="O1" s="80" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="P1" s="80" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="Q1" s="81"/>
       <c r="R1" s="81"/>
@@ -16973,7 +16987,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D2" s="36">
         <v>49.9</v>
@@ -16982,19 +16996,19 @@
         <v>1</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G2" s="36">
         <v>49.6</v>
       </c>
       <c r="H2" s="36" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="I2" s="36">
         <v>0.6</v>
       </c>
       <c r="J2" s="36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K2" s="36">
         <v>27.6</v>
@@ -17003,13 +17017,13 @@
         <v>1</v>
       </c>
       <c r="M2" s="36" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N2" s="36">
         <v>24.3</v>
       </c>
       <c r="O2" s="36" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P2" s="36">
         <v>23.1</v>
@@ -17023,7 +17037,7 @@
         <v>42</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D3" s="36">
         <v>60.4</v>
@@ -17032,13 +17046,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G3" s="36">
         <v>38.1</v>
       </c>
       <c r="J3" s="36" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K3" s="36">
         <v>53.3</v>
@@ -17047,13 +17061,13 @@
         <v>1</v>
       </c>
       <c r="M3" s="36" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N3" s="36">
         <v>15.8</v>
       </c>
       <c r="O3" s="36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="P3" s="36">
         <v>11.7</v>
@@ -17067,7 +17081,7 @@
         <v>52</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D4" s="36">
         <v>52.7</v>
@@ -17076,7 +17090,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G4" s="36">
         <v>47.2</v>
@@ -17090,7 +17104,7 @@
         <v>57</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K5" s="36">
         <v>32.5</v>
@@ -17099,13 +17113,13 @@
         <v>1</v>
       </c>
       <c r="M5" s="36" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="N5" s="36">
         <v>22.5</v>
       </c>
       <c r="O5" s="36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="P5" s="36">
         <v>22.3</v>
@@ -17119,7 +17133,7 @@
         <v>52</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K6" s="36">
         <v>45.9</v>
@@ -17128,13 +17142,13 @@
         <v>1</v>
       </c>
       <c r="M6" s="36" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="N6" s="36">
         <v>23.9</v>
       </c>
       <c r="O6" s="36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="P6" s="36">
         <v>21.4</v>
@@ -17148,7 +17162,7 @@
         <v>57</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D7" s="36">
         <v>73.5</v>
@@ -17157,7 +17171,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G7" s="36">
         <v>26.0</v>
@@ -17171,7 +17185,7 @@
         <v>69</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D8" s="36">
         <v>77.8</v>
@@ -17180,13 +17194,13 @@
         <v>1</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G8" s="36">
         <v>19.2</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K8" s="36">
         <v>43.4</v>
@@ -17195,13 +17209,13 @@
         <v>1</v>
       </c>
       <c r="M8" s="36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N8" s="36">
         <v>21.1</v>
       </c>
       <c r="O8" s="36" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P8" s="36">
         <v>18.7</v>
@@ -17215,7 +17229,7 @@
         <v>74</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K9" s="36">
         <v>36.4</v>
@@ -17224,13 +17238,13 @@
         <v>1</v>
       </c>
       <c r="M9" s="36" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N9" s="36">
         <v>33.5</v>
       </c>
       <c r="O9" s="36" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P9" s="36">
         <v>15.1</v>
@@ -17244,7 +17258,7 @@
         <v>78</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D10" s="36">
         <v>66.3</v>
@@ -17253,13 +17267,13 @@
         <v>1</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G10" s="36">
         <v>29.7</v>
       </c>
       <c r="J10" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K10" s="84">
         <v>32.8</v>
@@ -17268,13 +17282,13 @@
         <v>1</v>
       </c>
       <c r="M10" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N10" s="86">
         <v>30.5</v>
       </c>
       <c r="O10" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P10" s="86">
         <v>24.9</v>
@@ -17288,7 +17302,7 @@
         <v>84</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D11" s="36">
         <v>59.0</v>
@@ -17297,7 +17311,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G11" s="86">
         <v>40.3</v>
@@ -17311,7 +17325,7 @@
         <v>90</v>
       </c>
       <c r="C12" s="87" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D12" s="88">
         <v>71.3</v>
@@ -17320,13 +17334,13 @@
         <v>1</v>
       </c>
       <c r="F12" s="85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G12" s="86">
         <v>28.2</v>
       </c>
       <c r="J12" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K12" s="84">
         <v>38.8</v>
@@ -17335,13 +17349,13 @@
         <v>1</v>
       </c>
       <c r="M12" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="N12" s="86">
         <v>24.4</v>
       </c>
       <c r="O12" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="P12" s="86">
         <v>23.6</v>
@@ -17355,7 +17369,7 @@
         <v>96</v>
       </c>
       <c r="C13" s="87" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D13" s="88">
         <v>50.1</v>
@@ -17364,13 +17378,13 @@
         <v>1</v>
       </c>
       <c r="F13" s="85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G13" s="86">
         <v>48.7</v>
       </c>
       <c r="J13" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K13" s="84">
         <v>49.3</v>
@@ -17379,13 +17393,13 @@
         <v>1</v>
       </c>
       <c r="M13" s="85" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N13" s="86">
         <v>18.0</v>
       </c>
       <c r="O13" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P13" s="86">
         <v>17.9</v>
@@ -17399,7 +17413,7 @@
         <v>100</v>
       </c>
       <c r="C14" s="89" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D14" s="90">
         <v>61.6</v>
@@ -17408,13 +17422,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G14" s="86">
         <v>38.4</v>
       </c>
       <c r="J14" s="91" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="K14" s="92">
         <v>36.5</v>
@@ -17423,13 +17437,13 @@
         <v>1</v>
       </c>
       <c r="M14" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N14" s="86">
         <v>29.0</v>
       </c>
       <c r="O14" s="85" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="P14" s="86">
         <v>21.3</v>
@@ -17443,7 +17457,7 @@
         <v>105</v>
       </c>
       <c r="C15" s="89" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D15" s="90">
         <v>51.9</v>
@@ -17452,13 +17466,13 @@
         <v>1</v>
       </c>
       <c r="F15" s="85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G15" s="86">
         <v>41.5</v>
       </c>
       <c r="J15" s="93" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K15" s="94">
         <v>34.4</v>
@@ -17467,13 +17481,13 @@
         <v>1</v>
       </c>
       <c r="M15" s="85" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N15" s="86">
         <v>28.3</v>
       </c>
       <c r="O15" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P15" s="86">
         <v>26.0</v>
@@ -17487,7 +17501,7 @@
         <v>108</v>
       </c>
       <c r="C16" s="87" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D16" s="88">
         <v>66.1</v>
@@ -17496,13 +17510,13 @@
         <v>1</v>
       </c>
       <c r="F16" s="85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G16" s="86">
         <v>32.4</v>
       </c>
       <c r="J16" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K16" s="84">
         <v>38.9</v>
@@ -17511,13 +17525,13 @@
         <v>1</v>
       </c>
       <c r="M16" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N16" s="86">
         <v>24.7</v>
       </c>
       <c r="O16" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P16" s="86">
         <v>21.2</v>
@@ -17531,7 +17545,7 @@
         <v>112</v>
       </c>
       <c r="C17" s="87" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D17" s="88">
         <v>65.2</v>
@@ -17540,13 +17554,13 @@
         <v>1</v>
       </c>
       <c r="F17" s="85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G17" s="86">
         <v>33.2</v>
       </c>
       <c r="J17" s="93" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K17" s="94">
         <v>43.8</v>
@@ -17555,13 +17569,13 @@
         <v>1</v>
       </c>
       <c r="M17" s="85" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N17" s="86">
         <v>26.8</v>
       </c>
       <c r="O17" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P17" s="86">
         <v>17.7</v>
@@ -17575,7 +17589,7 @@
         <v>116</v>
       </c>
       <c r="C18" s="89" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D18" s="90">
         <v>86.1</v>
@@ -17584,13 +17598,13 @@
         <v>1</v>
       </c>
       <c r="F18" s="85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G18" s="86">
         <v>13.6</v>
       </c>
       <c r="J18" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K18" s="84">
         <v>32.7</v>
@@ -17599,13 +17613,13 @@
         <v>1</v>
       </c>
       <c r="M18" s="85" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N18" s="86">
         <v>30.4</v>
       </c>
       <c r="O18" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P18" s="86">
         <v>19.3</v>
@@ -17619,7 +17633,7 @@
         <v>121</v>
       </c>
       <c r="C19" s="87" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D19" s="88">
         <v>64.3</v>
@@ -17628,13 +17642,13 @@
         <v>1</v>
       </c>
       <c r="F19" s="85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G19" s="86">
         <v>35.2</v>
       </c>
       <c r="J19" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K19" s="84">
         <v>34.7</v>
@@ -17643,13 +17657,13 @@
         <v>1</v>
       </c>
       <c r="M19" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="N19" s="86">
         <v>31.9</v>
       </c>
       <c r="O19" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="P19" s="86">
         <v>16.9</v>
@@ -17663,7 +17677,7 @@
         <v>130</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D20" s="95">
         <v>73.0</v>
@@ -17672,7 +17686,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="95" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G20" s="95">
         <v>27.0</v>
@@ -17686,7 +17700,7 @@
         <v>141</v>
       </c>
       <c r="C21" s="89" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D21" s="90">
         <v>67.7</v>
@@ -17695,13 +17709,13 @@
         <v>1</v>
       </c>
       <c r="F21" s="85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G21" s="86">
         <v>32.3</v>
       </c>
       <c r="J21" s="93" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K21" s="94">
         <v>48.2</v>
@@ -17710,13 +17724,13 @@
         <v>1</v>
       </c>
       <c r="M21" s="85" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N21" s="86">
         <v>23.3</v>
       </c>
       <c r="O21" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P21" s="86">
         <v>16.7</v>
@@ -17730,7 +17744,7 @@
         <v>145</v>
       </c>
       <c r="J22" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K22" s="84">
         <v>35.9</v>
@@ -17739,13 +17753,13 @@
         <v>1</v>
       </c>
       <c r="M22" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N22" s="86">
         <v>31.6</v>
       </c>
       <c r="O22" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P22" s="86">
         <v>16.4</v>
@@ -17759,7 +17773,7 @@
         <v>150</v>
       </c>
       <c r="C23" s="87" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D23" s="88">
         <v>71.1</v>
@@ -17768,13 +17782,13 @@
         <v>1</v>
       </c>
       <c r="F23" s="85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G23" s="86">
         <v>23.2</v>
       </c>
       <c r="J23" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K23" s="84">
         <v>41.4</v>
@@ -17783,13 +17797,13 @@
         <v>1</v>
       </c>
       <c r="M23" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N23" s="86">
         <v>37.8</v>
       </c>
       <c r="O23" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P23" s="86">
         <v>11.2</v>
@@ -17803,7 +17817,7 @@
         <v>153</v>
       </c>
       <c r="J24" s="93" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K24" s="94">
         <v>45.9</v>
@@ -17812,13 +17826,13 @@
         <v>1</v>
       </c>
       <c r="M24" s="85" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N24" s="86">
         <v>32.6</v>
       </c>
       <c r="O24" s="85" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="P24" s="86">
         <v>12.2</v>
@@ -17832,7 +17846,7 @@
         <v>156</v>
       </c>
       <c r="C25" s="89" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D25" s="90">
         <v>57.1</v>
@@ -17841,7 +17855,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G25" s="86">
         <v>42.9</v>
@@ -20800,13 +20814,13 @@
         <v>15</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>23</v>
@@ -20839,7 +20853,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
@@ -20855,14 +20869,14 @@
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="25" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="24"/>
       <c r="G3" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="4">
@@ -20874,14 +20888,14 @@
       </c>
       <c r="C4" s="25"/>
       <c r="D4" s="25" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E4" s="25" t="s">
         <v>33</v>
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5">
@@ -20892,7 +20906,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -20908,14 +20922,14 @@
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>43</v>
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7">
@@ -20927,14 +20941,14 @@
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="31" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>43</v>
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8">
@@ -20959,14 +20973,14 @@
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="25" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>53</v>
       </c>
       <c r="F9" s="24"/>
       <c r="G9" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10">
@@ -20978,14 +20992,14 @@
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="31" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>58</v>
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11">
@@ -21010,14 +21024,14 @@
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="25" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>53</v>
       </c>
       <c r="F12" s="24"/>
       <c r="G12" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="13">
@@ -21042,14 +21056,14 @@
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="31" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="24"/>
       <c r="G14" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="15">
@@ -21078,14 +21092,14 @@
       </c>
       <c r="C16" s="31"/>
       <c r="D16" s="31" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>70</v>
       </c>
       <c r="F16" s="24"/>
       <c r="G16" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17">
@@ -21097,14 +21111,14 @@
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="31" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>70</v>
       </c>
       <c r="F17" s="24"/>
       <c r="G17" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="18">
@@ -21116,14 +21130,14 @@
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="25" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>75</v>
       </c>
       <c r="F18" s="24"/>
       <c r="G18" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="19">
@@ -21135,14 +21149,14 @@
       </c>
       <c r="C19" s="48"/>
       <c r="D19" s="48" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E19" s="38" t="s">
         <v>131</v>
       </c>
       <c r="F19" s="37"/>
       <c r="G19" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="20">
@@ -21154,14 +21168,14 @@
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>79</v>
       </c>
       <c r="F20" s="24"/>
       <c r="G20" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="21">
@@ -21173,14 +21187,14 @@
       </c>
       <c r="C21" s="31"/>
       <c r="D21" s="31" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>79</v>
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="22">
@@ -21192,14 +21206,14 @@
       </c>
       <c r="C22" s="38"/>
       <c r="D22" s="38" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E22" s="38" t="s">
         <v>85</v>
       </c>
       <c r="F22" s="37"/>
       <c r="G22" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="23">
@@ -21211,14 +21225,14 @@
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="31" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>85</v>
       </c>
       <c r="F23" s="24"/>
       <c r="G23" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="24">
@@ -21230,14 +21244,14 @@
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="31" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F24" s="24"/>
       <c r="G24" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25">
@@ -21249,14 +21263,14 @@
       </c>
       <c r="C25" s="31"/>
       <c r="D25" s="31" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26">
@@ -21268,14 +21282,14 @@
       </c>
       <c r="C26" s="31"/>
       <c r="D26" s="31" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>97</v>
       </c>
       <c r="F26" s="24"/>
       <c r="G26" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="27">
@@ -21287,14 +21301,14 @@
       </c>
       <c r="C27" s="31"/>
       <c r="D27" s="31" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>97</v>
       </c>
       <c r="F27" s="24"/>
       <c r="G27" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="28">
@@ -21306,14 +21320,14 @@
       </c>
       <c r="C28" s="31"/>
       <c r="D28" s="31" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E28" s="25" t="s">
         <v>101</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="29">
@@ -21325,14 +21339,14 @@
       </c>
       <c r="C29" s="31"/>
       <c r="D29" s="31" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E29" s="25" t="s">
         <v>101</v>
       </c>
       <c r="F29" s="24"/>
       <c r="G29" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="30">
@@ -21344,14 +21358,14 @@
       </c>
       <c r="C30" s="38"/>
       <c r="D30" s="38" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F30" s="37"/>
       <c r="G30" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31">
@@ -21363,14 +21377,14 @@
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F31" s="24"/>
       <c r="G31" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="32">
@@ -21382,14 +21396,14 @@
       </c>
       <c r="C32" s="31"/>
       <c r="D32" s="31" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E32" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F32" s="24"/>
       <c r="G32" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="33">
@@ -21401,14 +21415,14 @@
       </c>
       <c r="C33" s="31"/>
       <c r="D33" s="31" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>109</v>
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="34">
@@ -21420,14 +21434,14 @@
       </c>
       <c r="C34" s="31"/>
       <c r="D34" s="31" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E34" s="25" t="s">
         <v>109</v>
       </c>
       <c r="F34" s="24"/>
       <c r="G34" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="35">
@@ -21439,14 +21453,14 @@
       </c>
       <c r="C35" s="31"/>
       <c r="D35" s="31" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E35" s="25" t="s">
         <v>113</v>
       </c>
       <c r="F35" s="24"/>
       <c r="G35" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="36">
@@ -21458,14 +21472,14 @@
       </c>
       <c r="C36" s="31"/>
       <c r="D36" s="31" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E36" s="25" t="s">
         <v>113</v>
       </c>
       <c r="F36" s="24"/>
       <c r="G36" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="37">
@@ -21477,14 +21491,14 @@
       </c>
       <c r="C37" s="31"/>
       <c r="D37" s="31" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>117</v>
       </c>
       <c r="F37" s="24"/>
       <c r="G37" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="38">
@@ -21496,14 +21510,14 @@
       </c>
       <c r="C38" s="31"/>
       <c r="D38" s="31" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>117</v>
       </c>
       <c r="F38" s="24"/>
       <c r="G38" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="39">
@@ -21515,14 +21529,14 @@
       </c>
       <c r="C39" s="31"/>
       <c r="D39" s="31" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>122</v>
       </c>
       <c r="F39" s="24"/>
       <c r="G39" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="40">
@@ -21534,14 +21548,14 @@
       </c>
       <c r="C40" s="31"/>
       <c r="D40" s="31" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E40" s="25" t="s">
         <v>122</v>
       </c>
       <c r="F40" s="24"/>
       <c r="G40" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="41">
@@ -21553,14 +21567,14 @@
       </c>
       <c r="C41" s="38"/>
       <c r="D41" s="38" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E41" s="38" t="s">
         <v>127</v>
       </c>
       <c r="F41" s="37"/>
       <c r="G41" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="42">
@@ -21568,7 +21582,7 @@
         <v>27</v>
       </c>
       <c r="B42" s="100" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21"/>
@@ -21585,14 +21599,14 @@
       </c>
       <c r="C43" s="31"/>
       <c r="D43" s="31" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E43" s="25" t="s">
         <v>142</v>
       </c>
       <c r="F43" s="24"/>
       <c r="G43" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="44">
@@ -21604,14 +21618,14 @@
       </c>
       <c r="C44" s="31"/>
       <c r="D44" s="31" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E44" s="25" t="s">
         <v>142</v>
       </c>
       <c r="F44" s="24"/>
       <c r="G44" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="45">
@@ -21623,14 +21637,14 @@
       </c>
       <c r="C45" s="31"/>
       <c r="D45" s="31" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E45" s="25" t="s">
         <v>146</v>
       </c>
       <c r="F45" s="101"/>
       <c r="G45" s="101" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="46">
@@ -21642,14 +21656,14 @@
       </c>
       <c r="C46" s="31"/>
       <c r="D46" s="31" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E46" s="25" t="s">
         <v>151</v>
       </c>
       <c r="F46" s="101"/>
       <c r="G46" s="101" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="47">
@@ -21661,14 +21675,14 @@
       </c>
       <c r="C47" s="31"/>
       <c r="D47" s="31" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E47" s="25" t="s">
         <v>151</v>
       </c>
       <c r="F47" s="101"/>
       <c r="G47" s="101" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="48">
@@ -21680,14 +21694,14 @@
       </c>
       <c r="C48" s="31"/>
       <c r="D48" s="31" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E48" s="25" t="s">
         <v>154</v>
       </c>
       <c r="F48" s="101"/>
       <c r="G48" s="101" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="49">
@@ -21699,14 +21713,14 @@
       </c>
       <c r="C49" s="31"/>
       <c r="D49" s="31" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E49" s="25" t="s">
         <v>157</v>
       </c>
       <c r="F49" s="24"/>
       <c r="G49" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="50">
@@ -21714,7 +21728,7 @@
         <v>27</v>
       </c>
       <c r="B50" s="100" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21"/>
@@ -21731,14 +21745,14 @@
       </c>
       <c r="C51" s="31"/>
       <c r="D51" s="31" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E51" s="25" t="s">
         <v>154</v>
       </c>
       <c r="F51" s="24"/>
       <c r="G51" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="52">
@@ -21750,14 +21764,14 @@
       </c>
       <c r="C52" s="31"/>
       <c r="D52" s="31" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E52" s="25" t="s">
         <v>163</v>
       </c>
       <c r="F52" s="24"/>
       <c r="G52" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="53">
@@ -21765,7 +21779,7 @@
         <v>27</v>
       </c>
       <c r="B53" s="100" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
@@ -21778,18 +21792,18 @@
         <v>15</v>
       </c>
       <c r="B54" s="98" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C54" s="31"/>
       <c r="D54" s="31" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F54" s="24"/>
       <c r="G54" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="55">
@@ -21797,18 +21811,18 @@
         <v>15</v>
       </c>
       <c r="B55" s="98" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C55" s="31"/>
       <c r="D55" s="31" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F55" s="24"/>
       <c r="G55" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="56">
@@ -21816,18 +21830,18 @@
         <v>15</v>
       </c>
       <c r="B56" s="99" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C56" s="38"/>
       <c r="D56" s="38" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E56" s="38" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F56" s="37"/>
       <c r="G56" s="37" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="57">
@@ -21835,18 +21849,18 @@
         <v>15</v>
       </c>
       <c r="B57" s="98" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C57" s="31"/>
       <c r="D57" s="31" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E57" s="25" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F57" s="24"/>
       <c r="G57" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="58">
@@ -21854,18 +21868,18 @@
         <v>15</v>
       </c>
       <c r="B58" s="98" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C58" s="31"/>
       <c r="D58" s="31" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E58" s="25" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F58" s="24"/>
       <c r="G58" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="59">
@@ -21873,18 +21887,18 @@
         <v>15</v>
       </c>
       <c r="B59" s="98" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C59" s="31"/>
       <c r="D59" s="31" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E59" s="25" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F59" s="24"/>
       <c r="G59" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="60">
@@ -21892,18 +21906,18 @@
         <v>15</v>
       </c>
       <c r="B60" s="98" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C60" s="31"/>
       <c r="D60" s="31" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E60" s="25" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F60" s="24"/>
       <c r="G60" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="61">
@@ -21911,7 +21925,7 @@
         <v>27</v>
       </c>
       <c r="B61" s="100" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C61" s="21"/>
       <c r="D61" s="21"/>
@@ -21924,18 +21938,18 @@
         <v>15</v>
       </c>
       <c r="B62" s="98" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C62" s="25"/>
       <c r="D62" s="25" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E62" s="25" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F62" s="24"/>
       <c r="G62" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="63">
@@ -21943,18 +21957,18 @@
         <v>15</v>
       </c>
       <c r="B63" s="99" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C63" s="38"/>
       <c r="D63" s="38" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E63" s="38" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F63" s="37"/>
       <c r="G63" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="64">
@@ -21962,18 +21976,18 @@
         <v>15</v>
       </c>
       <c r="B64" s="98" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C64" s="31"/>
       <c r="D64" s="31" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E64" s="25" t="s">
         <v>127</v>
       </c>
       <c r="F64" s="24"/>
       <c r="G64" s="24" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="65">
@@ -21981,10 +21995,10 @@
         <v>27</v>
       </c>
       <c r="B65" s="100" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D65" s="17"/>
       <c r="E65" s="17"/>
@@ -21996,18 +22010,18 @@
         <v>15</v>
       </c>
       <c r="B66" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C66" s="31"/>
       <c r="D66" s="31" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E66" s="25" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F66" s="24"/>
       <c r="G66" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="67">
@@ -22015,18 +22029,18 @@
         <v>15</v>
       </c>
       <c r="B67" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C67" s="31"/>
       <c r="D67" s="31" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E67" s="25" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F67" s="24"/>
       <c r="G67" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="68">
@@ -22034,18 +22048,18 @@
         <v>15</v>
       </c>
       <c r="B68" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C68" s="31"/>
       <c r="D68" s="31" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E68" s="25" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F68" s="24"/>
       <c r="G68" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="69">
@@ -22053,18 +22067,18 @@
         <v>15</v>
       </c>
       <c r="B69" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C69" s="31"/>
       <c r="D69" s="31" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E69" s="25" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F69" s="24"/>
       <c r="G69" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="70">
@@ -22072,18 +22086,18 @@
         <v>15</v>
       </c>
       <c r="B70" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C70" s="31"/>
       <c r="D70" s="31" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E70" s="25" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F70" s="24"/>
       <c r="G70" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="71">
@@ -22091,18 +22105,18 @@
         <v>15</v>
       </c>
       <c r="B71" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="31" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E71" s="25" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F71" s="24"/>
       <c r="G71" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="72">
@@ -22110,18 +22124,18 @@
         <v>15</v>
       </c>
       <c r="B72" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C72" s="31"/>
       <c r="D72" s="31" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E72" s="25" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F72" s="24"/>
       <c r="G72" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="73">
@@ -22129,18 +22143,18 @@
         <v>15</v>
       </c>
       <c r="B73" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C73" s="31"/>
       <c r="D73" s="31" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E73" s="25" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F73" s="24"/>
       <c r="G73" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="74">
@@ -22148,18 +22162,18 @@
         <v>15</v>
       </c>
       <c r="B74" s="99" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C74" s="38"/>
       <c r="D74" s="38" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E74" s="38" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F74" s="37"/>
       <c r="G74" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="75">
@@ -22167,18 +22181,18 @@
         <v>15</v>
       </c>
       <c r="B75" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C75" s="31"/>
       <c r="D75" s="31" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E75" s="25" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F75" s="24"/>
       <c r="G75" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="76">
@@ -22186,18 +22200,18 @@
         <v>15</v>
       </c>
       <c r="B76" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C76" s="31"/>
       <c r="D76" s="31" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E76" s="25" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F76" s="24"/>
       <c r="G76" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="77">
@@ -22205,7 +22219,7 @@
         <v>27</v>
       </c>
       <c r="B77" s="100" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C77" s="21"/>
       <c r="D77" s="21"/>
@@ -22218,18 +22232,18 @@
         <v>15</v>
       </c>
       <c r="B78" s="99" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C78" s="38"/>
       <c r="D78" s="38" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E78" s="38" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F78" s="37"/>
       <c r="G78" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="79">
@@ -22237,7 +22251,7 @@
         <v>27</v>
       </c>
       <c r="B79" s="100" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C79" s="21"/>
       <c r="D79" s="21"/>
@@ -22250,18 +22264,18 @@
         <v>15</v>
       </c>
       <c r="B80" s="99" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C80" s="38"/>
       <c r="D80" s="38" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E80" s="38" t="s">
         <v>131</v>
       </c>
       <c r="F80" s="37"/>
       <c r="G80" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="81">
@@ -22269,18 +22283,18 @@
         <v>15</v>
       </c>
       <c r="B81" s="98" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C81" s="31"/>
       <c r="D81" s="31" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E81" s="25" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F81" s="24"/>
       <c r="G81" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="82">
@@ -22288,18 +22302,18 @@
         <v>15</v>
       </c>
       <c r="B82" s="98" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C82" s="31"/>
       <c r="D82" s="31" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E82" s="25" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F82" s="24"/>
       <c r="G82" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="83">
@@ -22307,18 +22321,18 @@
         <v>15</v>
       </c>
       <c r="B83" s="98" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C83" s="25"/>
       <c r="D83" s="25" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="E83" s="25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F83" s="24"/>
       <c r="G83" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="84">
@@ -22326,18 +22340,18 @@
         <v>15</v>
       </c>
       <c r="B84" s="98" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C84" s="25"/>
       <c r="D84" s="25" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E84" s="25" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F84" s="24"/>
       <c r="G84" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="85">
@@ -22345,16 +22359,16 @@
         <v>15</v>
       </c>
       <c r="B85" s="98" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C85" s="25"/>
       <c r="D85" s="25" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E85" s="31"/>
       <c r="F85" s="24"/>
       <c r="G85" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="86">
@@ -22362,7 +22376,7 @@
         <v>27</v>
       </c>
       <c r="B86" s="100" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C86" s="21"/>
       <c r="D86" s="21"/>
@@ -22375,18 +22389,18 @@
         <v>15</v>
       </c>
       <c r="B87" s="98" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C87" s="25"/>
       <c r="D87" s="25" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E87" s="25" t="s">
         <v>75</v>
       </c>
       <c r="F87" s="24"/>
       <c r="G87" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="88">
@@ -22394,18 +22408,18 @@
         <v>15</v>
       </c>
       <c r="B88" s="98" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C88" s="25"/>
       <c r="D88" s="25" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E88" s="25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F88" s="24"/>
       <c r="G88" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="89">
@@ -22413,18 +22427,18 @@
         <v>15</v>
       </c>
       <c r="B89" s="98" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C89" s="31"/>
       <c r="D89" s="31" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E89" s="25" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F89" s="24"/>
       <c r="G89" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="90">
@@ -22432,7 +22446,7 @@
         <v>27</v>
       </c>
       <c r="B90" s="100" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C90" s="21"/>
       <c r="D90" s="21"/>
@@ -22445,18 +22459,18 @@
         <v>15</v>
       </c>
       <c r="B91" s="98" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C91" s="31"/>
       <c r="D91" s="31" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E91" s="25" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F91" s="24"/>
       <c r="G91" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="92">
@@ -22464,18 +22478,18 @@
         <v>15</v>
       </c>
       <c r="B92" s="98" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C92" s="31"/>
       <c r="D92" s="31" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E92" s="25" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F92" s="24"/>
       <c r="G92" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="93">
@@ -22483,7 +22497,7 @@
         <v>27</v>
       </c>
       <c r="B93" s="100" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C93" s="21"/>
       <c r="D93" s="21"/>
@@ -22496,18 +22510,18 @@
         <v>15</v>
       </c>
       <c r="B94" s="98" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C94" s="25"/>
       <c r="D94" s="25" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E94" s="25" t="s">
         <v>127</v>
       </c>
       <c r="F94" s="24"/>
       <c r="G94" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="95">
@@ -22515,7 +22529,7 @@
         <v>27</v>
       </c>
       <c r="B95" s="100" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C95" s="21"/>
       <c r="D95" s="21"/>
@@ -22528,18 +22542,18 @@
         <v>15</v>
       </c>
       <c r="B96" s="98" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C96" s="31"/>
       <c r="D96" s="31" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E96" s="25" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F96" s="24"/>
       <c r="G96" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="97">
@@ -22547,18 +22561,18 @@
         <v>15</v>
       </c>
       <c r="B97" s="98" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C97" s="31"/>
       <c r="D97" s="31" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E97" s="25" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F97" s="24"/>
       <c r="G97" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="98">
@@ -22566,7 +22580,7 @@
         <v>27</v>
       </c>
       <c r="B98" s="100" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C98" s="21"/>
       <c r="D98" s="21"/>
@@ -22579,18 +22593,18 @@
         <v>15</v>
       </c>
       <c r="B99" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C99" s="31"/>
       <c r="D99" s="31" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E99" s="25" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F99" s="24"/>
       <c r="G99" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="100">
@@ -22598,18 +22612,18 @@
         <v>15</v>
       </c>
       <c r="B100" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C100" s="31"/>
       <c r="D100" s="31" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E100" s="25" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F100" s="24"/>
       <c r="G100" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="101">
@@ -22617,18 +22631,18 @@
         <v>15</v>
       </c>
       <c r="B101" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C101" s="31"/>
       <c r="D101" s="31" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E101" s="25" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F101" s="24"/>
       <c r="G101" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="102">
@@ -22636,18 +22650,18 @@
         <v>15</v>
       </c>
       <c r="B102" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C102" s="31"/>
       <c r="D102" s="31" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E102" s="25" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F102" s="24"/>
       <c r="G102" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="103">
@@ -22655,18 +22669,18 @@
         <v>15</v>
       </c>
       <c r="B103" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C103" s="31"/>
       <c r="D103" s="31" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E103" s="25" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F103" s="24"/>
       <c r="G103" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="104">
@@ -22674,18 +22688,18 @@
         <v>15</v>
       </c>
       <c r="B104" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C104" s="31"/>
       <c r="D104" s="31" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E104" s="25" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F104" s="24"/>
       <c r="G104" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="105">
@@ -22693,18 +22707,18 @@
         <v>15</v>
       </c>
       <c r="B105" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C105" s="31"/>
       <c r="D105" s="31" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E105" s="25" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F105" s="24"/>
       <c r="G105" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="106">
@@ -22712,18 +22726,18 @@
         <v>15</v>
       </c>
       <c r="B106" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C106" s="31"/>
       <c r="D106" s="31" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E106" s="25" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F106" s="24"/>
       <c r="G106" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="107">
@@ -22731,18 +22745,18 @@
         <v>15</v>
       </c>
       <c r="B107" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C107" s="31"/>
       <c r="D107" s="31" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E107" s="25" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F107" s="24"/>
       <c r="G107" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="108">
@@ -22750,18 +22764,18 @@
         <v>15</v>
       </c>
       <c r="B108" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C108" s="31"/>
       <c r="D108" s="31" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="E108" s="25" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F108" s="24"/>
       <c r="G108" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="109">
@@ -22769,7 +22783,7 @@
         <v>27</v>
       </c>
       <c r="B109" s="100" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C109" s="21"/>
       <c r="D109" s="21"/>
@@ -22782,18 +22796,18 @@
         <v>15</v>
       </c>
       <c r="B110" s="98" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C110" s="31"/>
       <c r="D110" s="31" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E110" s="25" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F110" s="24"/>
       <c r="G110" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="111">
@@ -22801,18 +22815,18 @@
         <v>15</v>
       </c>
       <c r="B111" s="98" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C111" s="31"/>
       <c r="D111" s="31" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E111" s="25" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F111" s="24"/>
       <c r="G111" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="112">
@@ -22820,7 +22834,7 @@
         <v>27</v>
       </c>
       <c r="B112" s="100" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C112" s="21"/>
       <c r="D112" s="21"/>
@@ -22833,18 +22847,18 @@
         <v>15</v>
       </c>
       <c r="B113" s="99" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C113" s="38"/>
       <c r="D113" s="38" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E113" s="38" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F113" s="37"/>
       <c r="G113" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="114">
@@ -22852,7 +22866,7 @@
         <v>27</v>
       </c>
       <c r="B114" s="100" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C114" s="21"/>
       <c r="D114" s="21"/>
@@ -22865,18 +22879,18 @@
         <v>15</v>
       </c>
       <c r="B115" s="98" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C115" s="31"/>
       <c r="D115" s="31" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="E115" s="25" t="s">
         <v>157</v>
       </c>
       <c r="F115" s="24"/>
       <c r="G115" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="116">
@@ -22884,18 +22898,18 @@
         <v>15</v>
       </c>
       <c r="B116" s="98" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C116" s="25"/>
       <c r="D116" s="25" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E116" s="25" t="s">
         <v>157</v>
       </c>
       <c r="F116" s="24"/>
       <c r="G116" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="117">
@@ -22903,18 +22917,18 @@
         <v>15</v>
       </c>
       <c r="B117" s="98" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C117" s="31"/>
       <c r="D117" s="31" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="E117" s="25" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F117" s="24"/>
       <c r="G117" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="118">
@@ -22922,18 +22936,18 @@
         <v>15</v>
       </c>
       <c r="B118" s="98" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C118" s="31"/>
       <c r="D118" s="31" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E118" s="25" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F118" s="24"/>
       <c r="G118" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="119">
@@ -22941,7 +22955,7 @@
         <v>27</v>
       </c>
       <c r="B119" s="100" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C119" s="21"/>
       <c r="D119" s="21"/>
@@ -22954,18 +22968,18 @@
         <v>15</v>
       </c>
       <c r="B120" s="98" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C120" s="31"/>
       <c r="D120" s="31" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E120" s="25" t="s">
         <v>146</v>
       </c>
       <c r="F120" s="24"/>
       <c r="G120" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="121">
@@ -22973,18 +22987,18 @@
         <v>15</v>
       </c>
       <c r="B121" s="98" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C121" s="31"/>
       <c r="D121" s="31" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="E121" s="25" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F121" s="24"/>
       <c r="G121" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="122">
@@ -22992,18 +23006,18 @@
         <v>15</v>
       </c>
       <c r="B122" s="98" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C122" s="31"/>
       <c r="D122" s="31" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="E122" s="25" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F122" s="24"/>
       <c r="G122" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="123">
@@ -23011,7 +23025,7 @@
         <v>27</v>
       </c>
       <c r="B123" s="100" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C123" s="21"/>
       <c r="D123" s="21"/>
@@ -23024,18 +23038,18 @@
         <v>15</v>
       </c>
       <c r="B124" s="98" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C124" s="25"/>
       <c r="D124" s="25" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E124" s="25" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F124" s="24"/>
       <c r="G124" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="125">
@@ -23043,18 +23057,18 @@
         <v>15</v>
       </c>
       <c r="B125" s="98" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C125" s="31"/>
       <c r="D125" s="31" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E125" s="25" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F125" s="24"/>
       <c r="G125" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="126">
@@ -23062,7 +23076,7 @@
         <v>27</v>
       </c>
       <c r="B126" s="100" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C126" s="21"/>
       <c r="D126" s="21"/>
@@ -23075,18 +23089,18 @@
         <v>15</v>
       </c>
       <c r="B127" s="99" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C127" s="48"/>
       <c r="D127" s="48" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E127" s="38" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F127" s="37"/>
       <c r="G127" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="128">
@@ -23094,7 +23108,7 @@
         <v>27</v>
       </c>
       <c r="B128" s="102" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C128" s="21"/>
       <c r="D128" s="21"/>
@@ -23107,18 +23121,18 @@
         <v>15</v>
       </c>
       <c r="B129" s="103" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C129" s="63"/>
       <c r="D129" s="63" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E129" s="64" t="s">
         <v>163</v>
       </c>
       <c r="F129" s="62"/>
       <c r="G129" s="62" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="130">
@@ -23126,7 +23140,7 @@
         <v>27</v>
       </c>
       <c r="B130" s="100" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C130" s="21"/>
       <c r="D130" s="21"/>
@@ -23139,18 +23153,18 @@
         <v>15</v>
       </c>
       <c r="B131" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C131" s="31"/>
       <c r="D131" s="31" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E131" s="25" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F131" s="24"/>
       <c r="G131" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="132">
@@ -23158,18 +23172,18 @@
         <v>15</v>
       </c>
       <c r="B132" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C132" s="31"/>
       <c r="D132" s="31" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="E132" s="25" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F132" s="24"/>
       <c r="G132" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="133">
@@ -23177,18 +23191,18 @@
         <v>15</v>
       </c>
       <c r="B133" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C133" s="31"/>
       <c r="D133" s="31" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E133" s="25" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F133" s="24"/>
       <c r="G133" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="134">
@@ -23196,18 +23210,18 @@
         <v>15</v>
       </c>
       <c r="B134" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C134" s="31"/>
       <c r="D134" s="31" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E134" s="25" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F134" s="24"/>
       <c r="G134" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="135">
@@ -23215,18 +23229,18 @@
         <v>15</v>
       </c>
       <c r="B135" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C135" s="31"/>
       <c r="D135" s="31" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E135" s="25" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F135" s="24"/>
       <c r="G135" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="136">
@@ -23234,18 +23248,18 @@
         <v>15</v>
       </c>
       <c r="B136" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C136" s="31"/>
       <c r="D136" s="31" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E136" s="25" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F136" s="24"/>
       <c r="G136" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="137">
@@ -23253,18 +23267,18 @@
         <v>15</v>
       </c>
       <c r="B137" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C137" s="31"/>
       <c r="D137" s="31" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="E137" s="25" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F137" s="24"/>
       <c r="G137" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="138">
@@ -23272,18 +23286,18 @@
         <v>15</v>
       </c>
       <c r="B138" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C138" s="31"/>
       <c r="D138" s="31" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E138" s="25" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F138" s="24"/>
       <c r="G138" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="139">
@@ -23291,18 +23305,18 @@
         <v>15</v>
       </c>
       <c r="B139" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C139" s="31"/>
       <c r="D139" s="31" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E139" s="25" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F139" s="24"/>
       <c r="G139" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="140">
@@ -23310,18 +23324,18 @@
         <v>15</v>
       </c>
       <c r="B140" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C140" s="31"/>
       <c r="D140" s="31" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E140" s="25" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F140" s="24"/>
       <c r="G140" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="141">
@@ -23329,18 +23343,18 @@
         <v>15</v>
       </c>
       <c r="B141" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C141" s="31"/>
       <c r="D141" s="31" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E141" s="25" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F141" s="24"/>
       <c r="G141" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="142">
@@ -23348,7 +23362,7 @@
         <v>27</v>
       </c>
       <c r="B142" s="100" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C142" s="21"/>
       <c r="D142" s="21"/>
@@ -23361,18 +23375,18 @@
         <v>15</v>
       </c>
       <c r="B143" s="98" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C143" s="31"/>
       <c r="D143" s="31" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E143" s="25" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F143" s="24"/>
       <c r="G143" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="144">

</xml_diff>

<commit_message>
add route for results pr
</commit_message>
<xml_diff>
--- a/data/calendar.xlsx
+++ b/data/calendar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="482">
   <si>
     <t>key</t>
   </si>
@@ -513,6 +513,9 @@
   </si>
   <si>
     <t>Tuesday, March 8</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
   <si>
     <t>3/8/2016</t>
@@ -3555,6 +3558,12 @@
         <v>38</v>
       </c>
       <c r="L36" s="55"/>
+      <c r="M36" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="N36" s="49">
+        <v>42435.833333333336</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="23" t="s">
@@ -3583,6 +3592,8 @@
         <v>49</v>
       </c>
       <c r="L37" s="55"/>
+      <c r="M37" s="36"/>
+      <c r="N37" s="49"/>
     </row>
     <row r="38">
       <c r="A38" s="15" t="s">
@@ -3601,20 +3612,23 @@
       <c r="J38" s="20"/>
       <c r="K38" s="21"/>
       <c r="L38" s="55"/>
+      <c r="M38" s="36" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C39" s="31"/>
       <c r="D39" s="25" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F39" s="26"/>
       <c r="G39" s="33"/>
@@ -3623,7 +3637,7 @@
         <v>36</v>
       </c>
       <c r="J39" s="30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K39" s="23" t="s">
         <v>38</v>
@@ -3635,14 +3649,14 @@
         <v>15</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C40" s="31"/>
       <c r="D40" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F40" s="26"/>
       <c r="G40" s="46"/>
@@ -3663,21 +3677,21 @@
         <v>15</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C41" s="31"/>
       <c r="D41" s="25" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F41" s="26"/>
       <c r="G41" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H41" s="30" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I41" s="29" t="s">
         <v>47</v>
@@ -3695,21 +3709,21 @@
         <v>15</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C42" s="31"/>
       <c r="D42" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F42" s="26"/>
       <c r="G42" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I42" s="29" t="s">
         <v>47</v>
@@ -3727,7 +3741,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21"/>
@@ -3745,14 +3759,14 @@
         <v>15</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C44" s="25"/>
       <c r="D44" s="25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F44" s="26"/>
       <c r="G44" s="33"/>
@@ -3761,7 +3775,7 @@
         <v>36</v>
       </c>
       <c r="J44" s="30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K44" s="23" t="s">
         <v>38</v>
@@ -3773,7 +3787,7 @@
         <v>15</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C45" s="31"/>
       <c r="D45" s="25" t="s">
@@ -3786,13 +3800,13 @@
       <c r="G45" s="33"/>
       <c r="H45" s="34"/>
       <c r="I45" s="56" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J45" s="57" t="s">
         <v>129</v>
       </c>
       <c r="K45" s="24" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L45" s="55"/>
     </row>
@@ -3801,21 +3815,21 @@
         <v>15</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C46" s="38"/>
       <c r="D46" s="38" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E46" s="43" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F46" s="43"/>
       <c r="G46" s="39" t="s">
         <v>133</v>
       </c>
       <c r="H46" s="40" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I46" s="44"/>
       <c r="J46" s="45"/>
@@ -3829,7 +3843,7 @@
         <v>27</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="17"/>
@@ -3847,27 +3861,27 @@
         <v>15</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C48" s="31"/>
       <c r="D48" s="25" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F48" s="26"/>
       <c r="G48" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I48" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J48" s="30" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K48" s="23" t="s">
         <v>49</v>
@@ -3879,27 +3893,27 @@
         <v>15</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C49" s="31"/>
       <c r="D49" s="25" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F49" s="26"/>
       <c r="G49" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I49" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J49" s="30" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="K49" s="23" t="s">
         <v>49</v>
@@ -3911,21 +3925,21 @@
         <v>15</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="25" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F50" s="26"/>
       <c r="G50" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I50" s="29" t="s">
         <v>47</v>
@@ -3943,27 +3957,27 @@
         <v>15</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C51" s="31"/>
       <c r="D51" s="25" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F51" s="26"/>
       <c r="G51" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H51" s="30" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I51" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J51" s="30" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K51" s="23" t="s">
         <v>49</v>
@@ -3975,27 +3989,27 @@
         <v>15</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C52" s="31"/>
       <c r="D52" s="25" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F52" s="26"/>
       <c r="G52" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H52" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I52" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J52" s="30" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K52" s="23" t="s">
         <v>49</v>
@@ -4007,23 +4021,23 @@
         <v>15</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C53" s="38"/>
       <c r="D53" s="38" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E53" s="43" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F53" s="43"/>
       <c r="G53" s="44"/>
       <c r="H53" s="45"/>
       <c r="I53" s="39" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J53" s="40" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K53" s="41" t="s">
         <v>38</v>
@@ -4035,7 +4049,7 @@
         <v>27</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="21"/>
@@ -4053,23 +4067,23 @@
         <v>15</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C55" s="38"/>
       <c r="D55" s="38" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E55" s="43" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F55" s="43"/>
       <c r="G55" s="44"/>
       <c r="H55" s="45"/>
       <c r="I55" s="39" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J55" s="40" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K55" s="41" t="s">
         <v>38</v>
@@ -4081,7 +4095,7 @@
         <v>27</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C56" s="21"/>
       <c r="D56" s="21"/>
@@ -4099,21 +4113,21 @@
         <v>15</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C57" s="31"/>
       <c r="D57" s="25" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E57" s="26" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F57" s="26"/>
       <c r="G57" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H57" s="30" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I57" s="29" t="s">
         <v>47</v>
@@ -4131,21 +4145,21 @@
         <v>15</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C58" s="25"/>
       <c r="D58" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E58" s="26" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F58" s="26"/>
       <c r="G58" s="29" t="s">
         <v>34</v>
       </c>
       <c r="H58" s="30" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I58" s="33"/>
       <c r="J58" s="34"/>
@@ -4159,14 +4173,14 @@
         <v>15</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C59" s="25"/>
       <c r="D59" s="25" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E59" s="26" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F59" s="26"/>
       <c r="G59" s="29" t="s">
@@ -4191,7 +4205,7 @@
         <v>15</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C60" s="38"/>
       <c r="D60" s="38" t="s">
@@ -4204,10 +4218,10 @@
       <c r="G60" s="44"/>
       <c r="H60" s="45"/>
       <c r="I60" s="46" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J60" s="47" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K60" s="41" t="s">
         <v>38</v>
@@ -4219,7 +4233,7 @@
         <v>27</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C61" s="58"/>
       <c r="D61" s="21"/>
@@ -4237,7 +4251,7 @@
         <v>15</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C62" s="25"/>
       <c r="D62" s="25" t="s">
@@ -4251,7 +4265,7 @@
         <v>34</v>
       </c>
       <c r="H62" s="30" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I62" s="33"/>
       <c r="J62" s="34"/>
@@ -4265,21 +4279,21 @@
         <v>15</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C63" s="25"/>
       <c r="D63" s="25" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E63" s="26" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F63" s="26"/>
       <c r="G63" s="29" t="s">
         <v>34</v>
       </c>
       <c r="H63" s="30" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="I63" s="33"/>
       <c r="J63" s="34"/>
@@ -4293,21 +4307,21 @@
         <v>15</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C64" s="31"/>
       <c r="D64" s="25" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E64" s="26" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F64" s="26"/>
       <c r="G64" s="29" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H64" s="30" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I64" s="33"/>
       <c r="J64" s="34"/>
@@ -4321,7 +4335,7 @@
         <v>27</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C65" s="21"/>
       <c r="D65" s="21"/>
@@ -4339,21 +4353,21 @@
         <v>15</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C66" s="31"/>
       <c r="D66" s="25" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E66" s="26" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F66" s="26"/>
       <c r="G66" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H66" s="30" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="I66" s="59" t="s">
         <v>47</v>
@@ -4371,7 +4385,7 @@
         <v>27</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C67" s="21"/>
       <c r="D67" s="21"/>
@@ -4389,7 +4403,7 @@
         <v>15</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C68" s="25"/>
       <c r="D68" s="25" t="s">
@@ -4403,7 +4417,7 @@
         <v>34</v>
       </c>
       <c r="H68" s="30" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I68" s="33"/>
       <c r="J68" s="34"/>
@@ -4417,7 +4431,7 @@
         <v>27</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C69" s="21"/>
       <c r="D69" s="21"/>
@@ -4435,27 +4449,27 @@
         <v>15</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C70" s="31"/>
       <c r="D70" s="25" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E70" s="26" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F70" s="26"/>
       <c r="G70" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H70" s="30" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I70" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J70" s="30" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K70" s="23" t="s">
         <v>49</v>
@@ -4467,7 +4481,7 @@
         <v>27</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C71" s="21"/>
       <c r="D71" s="21"/>
@@ -4485,21 +4499,21 @@
         <v>15</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C72" s="31"/>
       <c r="D72" s="25" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E72" s="26" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F72" s="26"/>
       <c r="G72" s="59" t="s">
         <v>45</v>
       </c>
       <c r="H72" s="60" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I72" s="29" t="s">
         <v>47</v>
@@ -4517,21 +4531,21 @@
         <v>15</v>
       </c>
       <c r="B73" s="24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C73" s="31"/>
       <c r="D73" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E73" s="26" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F73" s="26"/>
       <c r="G73" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H73" s="30" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="I73" s="29" t="s">
         <v>47</v>
@@ -4549,21 +4563,21 @@
         <v>15</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C74" s="31"/>
       <c r="D74" s="25" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E74" s="26" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F74" s="26"/>
       <c r="G74" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H74" s="30" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I74" s="29" t="s">
         <v>45</v>
@@ -4581,27 +4595,27 @@
         <v>15</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C75" s="31"/>
       <c r="D75" s="25" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E75" s="26" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F75" s="26"/>
       <c r="G75" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H75" s="30" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I75" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J75" s="30" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="K75" s="23" t="s">
         <v>49</v>
@@ -4613,27 +4627,27 @@
         <v>15</v>
       </c>
       <c r="B76" s="24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C76" s="31"/>
       <c r="D76" s="25" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E76" s="26" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F76" s="26"/>
       <c r="G76" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H76" s="30" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I76" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J76" s="30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K76" s="23" t="s">
         <v>49</v>
@@ -4645,7 +4659,7 @@
         <v>27</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C77" s="21"/>
       <c r="D77" s="21"/>
@@ -4663,27 +4677,27 @@
         <v>15</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C78" s="31"/>
       <c r="D78" s="25" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E78" s="26" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F78" s="26"/>
       <c r="G78" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H78" s="30" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I78" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J78" s="30" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K78" s="23" t="s">
         <v>49</v>
@@ -4695,7 +4709,7 @@
         <v>27</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C79" s="21"/>
       <c r="D79" s="21"/>
@@ -4713,21 +4727,21 @@
         <v>15</v>
       </c>
       <c r="B80" s="37" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C80" s="38"/>
       <c r="D80" s="38" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E80" s="43" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F80" s="43"/>
       <c r="G80" s="39" t="s">
         <v>34</v>
       </c>
       <c r="H80" s="40" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I80" s="44"/>
       <c r="J80" s="45"/>
@@ -4741,7 +4755,7 @@
         <v>27</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C81" s="21"/>
       <c r="D81" s="21"/>
@@ -4759,7 +4773,7 @@
         <v>15</v>
       </c>
       <c r="B82" s="24" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C82" s="31"/>
       <c r="D82" s="25" t="s">
@@ -4770,7 +4784,7 @@
       </c>
       <c r="F82" s="26"/>
       <c r="G82" s="56" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H82" s="57" t="s">
         <v>37</v>
@@ -4779,7 +4793,7 @@
         <v>47</v>
       </c>
       <c r="J82" s="30" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K82" s="23" t="s">
         <v>49</v>
@@ -4791,14 +4805,14 @@
         <v>15</v>
       </c>
       <c r="B83" s="24" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C83" s="31"/>
       <c r="D83" s="25" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E83" s="26" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F83" s="26"/>
       <c r="G83" s="29" t="s">
@@ -4811,7 +4825,7 @@
         <v>47</v>
       </c>
       <c r="J83" s="30" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="K83" s="23" t="s">
         <v>49</v>
@@ -4823,7 +4837,7 @@
         <v>27</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C84" s="21"/>
       <c r="D84" s="21"/>
@@ -4841,7 +4855,7 @@
         <v>15</v>
       </c>
       <c r="B85" s="24" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C85" s="31"/>
       <c r="D85" s="25" t="s">
@@ -4855,7 +4869,7 @@
         <v>45</v>
       </c>
       <c r="H85" s="30" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="I85" s="33"/>
       <c r="J85" s="34"/>
@@ -4869,21 +4883,21 @@
         <v>15</v>
       </c>
       <c r="B86" s="24" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C86" s="31"/>
       <c r="D86" s="25" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E86" s="26" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F86" s="26"/>
       <c r="G86" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H86" s="30" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I86" s="29" t="s">
         <v>47</v>
@@ -4901,7 +4915,7 @@
         <v>27</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C87" s="21"/>
       <c r="D87" s="21"/>
@@ -4919,27 +4933,27 @@
         <v>15</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C88" s="25"/>
       <c r="D88" s="25" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F88" s="26"/>
       <c r="G88" s="56" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H88" s="57" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I88" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J88" s="30" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="K88" s="23" t="s">
         <v>49</v>
@@ -4951,7 +4965,7 @@
         <v>27</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C89" s="21"/>
       <c r="D89" s="21"/>
@@ -4969,21 +4983,21 @@
         <v>15</v>
       </c>
       <c r="B90" s="37" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C90" s="48"/>
       <c r="D90" s="38" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E90" s="43" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F90" s="43"/>
       <c r="G90" s="39" t="s">
         <v>133</v>
       </c>
       <c r="H90" s="40" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I90" s="44"/>
       <c r="J90" s="45"/>
@@ -4997,7 +5011,7 @@
         <v>27</v>
       </c>
       <c r="B91" s="61" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C91" s="21"/>
       <c r="D91" s="21"/>
@@ -5015,7 +5029,7 @@
         <v>15</v>
       </c>
       <c r="B92" s="62" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C92" s="63"/>
       <c r="D92" s="64" t="s">
@@ -5029,7 +5043,7 @@
         <v>34</v>
       </c>
       <c r="H92" s="67" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="I92" s="68"/>
       <c r="J92" s="69"/>
@@ -5043,7 +5057,7 @@
         <v>27</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C93" s="21"/>
       <c r="D93" s="21"/>
@@ -5061,27 +5075,27 @@
         <v>15</v>
       </c>
       <c r="B94" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C94" s="31"/>
       <c r="D94" s="25" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E94" s="26" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F94" s="26"/>
       <c r="G94" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H94" s="30" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="I94" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J94" s="30" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="K94" s="23" t="s">
         <v>49</v>
@@ -5093,27 +5107,27 @@
         <v>15</v>
       </c>
       <c r="B95" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C95" s="31"/>
       <c r="D95" s="25" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E95" s="26" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F95" s="26"/>
       <c r="G95" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H95" s="30" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I95" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J95" s="30" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K95" s="23" t="s">
         <v>49</v>
@@ -5125,27 +5139,27 @@
         <v>15</v>
       </c>
       <c r="B96" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C96" s="31"/>
       <c r="D96" s="25" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E96" s="26" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F96" s="26"/>
       <c r="G96" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H96" s="30" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I96" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J96" s="30" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K96" s="23" t="s">
         <v>49</v>
@@ -5157,14 +5171,14 @@
         <v>15</v>
       </c>
       <c r="B97" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C97" s="31"/>
       <c r="D97" s="25" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E97" s="26" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F97" s="26"/>
       <c r="G97" s="29" t="s">
@@ -5177,7 +5191,7 @@
         <v>47</v>
       </c>
       <c r="J97" s="30" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="K97" s="23" t="s">
         <v>49</v>
@@ -5189,14 +5203,14 @@
         <v>15</v>
       </c>
       <c r="B98" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C98" s="31"/>
       <c r="D98" s="25" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E98" s="26" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F98" s="26"/>
       <c r="G98" s="29" t="s">
@@ -5217,21 +5231,21 @@
         <v>15</v>
       </c>
       <c r="B99" s="24" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C99" s="31"/>
       <c r="D99" s="25" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E99" s="26" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F99" s="26"/>
       <c r="G99" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H99" s="30" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I99" s="29" t="s">
         <v>47</v>
@@ -5249,7 +5263,7 @@
         <v>27</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C100" s="21"/>
       <c r="D100" s="21"/>
@@ -5267,21 +5281,21 @@
         <v>15</v>
       </c>
       <c r="B101" s="24" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C101" s="31"/>
       <c r="D101" s="25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E101" s="26" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F101" s="26"/>
       <c r="G101" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H101" s="30" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="I101" s="33"/>
       <c r="J101" s="34"/>
@@ -16919,46 +16933,46 @@
         <v>16</v>
       </c>
       <c r="C1" s="80" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D1" s="80" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E1" s="80" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F1" s="80" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G1" s="80" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="H1" s="80" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="I1" s="80" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J1" s="80" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="K1" s="80" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="L1" s="80" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="M1" s="80" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="N1" s="80" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="O1" s="80" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="P1" s="80" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="Q1" s="81"/>
       <c r="R1" s="81"/>
@@ -16973,7 +16987,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D2" s="36">
         <v>49.9</v>
@@ -16982,19 +16996,19 @@
         <v>1</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G2" s="36">
         <v>49.6</v>
       </c>
       <c r="H2" s="36" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="I2" s="36">
         <v>0.6</v>
       </c>
       <c r="J2" s="36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K2" s="36">
         <v>27.6</v>
@@ -17003,13 +17017,13 @@
         <v>1</v>
       </c>
       <c r="M2" s="36" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N2" s="36">
         <v>24.3</v>
       </c>
       <c r="O2" s="36" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P2" s="36">
         <v>23.1</v>
@@ -17023,7 +17037,7 @@
         <v>42</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D3" s="36">
         <v>60.4</v>
@@ -17032,13 +17046,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G3" s="36">
         <v>38.1</v>
       </c>
       <c r="J3" s="36" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K3" s="36">
         <v>53.3</v>
@@ -17047,13 +17061,13 @@
         <v>1</v>
       </c>
       <c r="M3" s="36" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N3" s="36">
         <v>15.8</v>
       </c>
       <c r="O3" s="36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="P3" s="36">
         <v>11.7</v>
@@ -17067,7 +17081,7 @@
         <v>52</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D4" s="36">
         <v>52.7</v>
@@ -17076,7 +17090,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G4" s="36">
         <v>47.2</v>
@@ -17090,7 +17104,7 @@
         <v>57</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K5" s="36">
         <v>32.5</v>
@@ -17099,13 +17113,13 @@
         <v>1</v>
       </c>
       <c r="M5" s="36" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="N5" s="36">
         <v>22.5</v>
       </c>
       <c r="O5" s="36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="P5" s="36">
         <v>22.3</v>
@@ -17119,7 +17133,7 @@
         <v>52</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K6" s="36">
         <v>45.9</v>
@@ -17128,13 +17142,13 @@
         <v>1</v>
       </c>
       <c r="M6" s="36" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="N6" s="36">
         <v>23.9</v>
       </c>
       <c r="O6" s="36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="P6" s="36">
         <v>21.4</v>
@@ -17148,7 +17162,7 @@
         <v>57</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D7" s="36">
         <v>73.5</v>
@@ -17157,7 +17171,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G7" s="36">
         <v>26.0</v>
@@ -17171,7 +17185,7 @@
         <v>69</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D8" s="36">
         <v>77.8</v>
@@ -17180,13 +17194,13 @@
         <v>1</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G8" s="36">
         <v>19.2</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K8" s="36">
         <v>43.4</v>
@@ -17195,13 +17209,13 @@
         <v>1</v>
       </c>
       <c r="M8" s="36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N8" s="36">
         <v>21.1</v>
       </c>
       <c r="O8" s="36" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P8" s="36">
         <v>18.7</v>
@@ -17215,7 +17229,7 @@
         <v>74</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K9" s="36">
         <v>36.4</v>
@@ -17224,13 +17238,13 @@
         <v>1</v>
       </c>
       <c r="M9" s="36" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N9" s="36">
         <v>33.5</v>
       </c>
       <c r="O9" s="36" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P9" s="36">
         <v>15.1</v>
@@ -17244,7 +17258,7 @@
         <v>78</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D10" s="36">
         <v>66.3</v>
@@ -17253,13 +17267,13 @@
         <v>1</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G10" s="36">
         <v>29.7</v>
       </c>
       <c r="J10" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K10" s="84">
         <v>32.8</v>
@@ -17268,13 +17282,13 @@
         <v>1</v>
       </c>
       <c r="M10" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N10" s="86">
         <v>30.5</v>
       </c>
       <c r="O10" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P10" s="86">
         <v>24.9</v>
@@ -17288,7 +17302,7 @@
         <v>84</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D11" s="36">
         <v>59.0</v>
@@ -17297,7 +17311,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G11" s="86">
         <v>40.3</v>
@@ -17311,7 +17325,7 @@
         <v>90</v>
       </c>
       <c r="C12" s="87" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D12" s="88">
         <v>71.3</v>
@@ -17320,13 +17334,13 @@
         <v>1</v>
       </c>
       <c r="F12" s="85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G12" s="86">
         <v>28.2</v>
       </c>
       <c r="J12" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K12" s="84">
         <v>38.8</v>
@@ -17335,13 +17349,13 @@
         <v>1</v>
       </c>
       <c r="M12" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="N12" s="86">
         <v>24.4</v>
       </c>
       <c r="O12" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="P12" s="86">
         <v>23.6</v>
@@ -17355,7 +17369,7 @@
         <v>96</v>
       </c>
       <c r="C13" s="87" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D13" s="88">
         <v>50.1</v>
@@ -17364,13 +17378,13 @@
         <v>1</v>
       </c>
       <c r="F13" s="85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G13" s="86">
         <v>48.7</v>
       </c>
       <c r="J13" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K13" s="84">
         <v>49.3</v>
@@ -17379,13 +17393,13 @@
         <v>1</v>
       </c>
       <c r="M13" s="85" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N13" s="86">
         <v>18.0</v>
       </c>
       <c r="O13" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P13" s="86">
         <v>17.9</v>
@@ -17399,7 +17413,7 @@
         <v>100</v>
       </c>
       <c r="C14" s="89" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D14" s="90">
         <v>61.6</v>
@@ -17408,13 +17422,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G14" s="86">
         <v>38.4</v>
       </c>
       <c r="J14" s="91" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="K14" s="92">
         <v>36.5</v>
@@ -17423,13 +17437,13 @@
         <v>1</v>
       </c>
       <c r="M14" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N14" s="86">
         <v>29.0</v>
       </c>
       <c r="O14" s="85" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="P14" s="86">
         <v>21.3</v>
@@ -17443,7 +17457,7 @@
         <v>105</v>
       </c>
       <c r="C15" s="89" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D15" s="90">
         <v>51.9</v>
@@ -17452,13 +17466,13 @@
         <v>1</v>
       </c>
       <c r="F15" s="85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G15" s="86">
         <v>41.5</v>
       </c>
       <c r="J15" s="93" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K15" s="94">
         <v>34.4</v>
@@ -17467,13 +17481,13 @@
         <v>1</v>
       </c>
       <c r="M15" s="85" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N15" s="86">
         <v>28.3</v>
       </c>
       <c r="O15" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P15" s="86">
         <v>26.0</v>
@@ -17487,7 +17501,7 @@
         <v>108</v>
       </c>
       <c r="C16" s="87" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D16" s="88">
         <v>66.1</v>
@@ -17496,13 +17510,13 @@
         <v>1</v>
       </c>
       <c r="F16" s="85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G16" s="86">
         <v>32.4</v>
       </c>
       <c r="J16" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K16" s="84">
         <v>38.9</v>
@@ -17511,13 +17525,13 @@
         <v>1</v>
       </c>
       <c r="M16" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N16" s="86">
         <v>24.7</v>
       </c>
       <c r="O16" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P16" s="86">
         <v>21.2</v>
@@ -17531,7 +17545,7 @@
         <v>112</v>
       </c>
       <c r="C17" s="87" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D17" s="88">
         <v>65.2</v>
@@ -17540,13 +17554,13 @@
         <v>1</v>
       </c>
       <c r="F17" s="85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G17" s="86">
         <v>33.2</v>
       </c>
       <c r="J17" s="93" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K17" s="94">
         <v>43.8</v>
@@ -17555,13 +17569,13 @@
         <v>1</v>
       </c>
       <c r="M17" s="85" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N17" s="86">
         <v>26.8</v>
       </c>
       <c r="O17" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P17" s="86">
         <v>17.7</v>
@@ -17575,7 +17589,7 @@
         <v>116</v>
       </c>
       <c r="C18" s="89" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D18" s="90">
         <v>86.1</v>
@@ -17584,13 +17598,13 @@
         <v>1</v>
       </c>
       <c r="F18" s="85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G18" s="86">
         <v>13.6</v>
       </c>
       <c r="J18" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K18" s="84">
         <v>32.7</v>
@@ -17599,13 +17613,13 @@
         <v>1</v>
       </c>
       <c r="M18" s="85" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N18" s="86">
         <v>30.4</v>
       </c>
       <c r="O18" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P18" s="86">
         <v>19.3</v>
@@ -17619,7 +17633,7 @@
         <v>121</v>
       </c>
       <c r="C19" s="87" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D19" s="88">
         <v>64.3</v>
@@ -17628,13 +17642,13 @@
         <v>1</v>
       </c>
       <c r="F19" s="85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G19" s="86">
         <v>35.2</v>
       </c>
       <c r="J19" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K19" s="84">
         <v>34.7</v>
@@ -17643,13 +17657,13 @@
         <v>1</v>
       </c>
       <c r="M19" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="N19" s="86">
         <v>31.9</v>
       </c>
       <c r="O19" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="P19" s="86">
         <v>16.9</v>
@@ -17663,7 +17677,7 @@
         <v>130</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D20" s="95">
         <v>73.0</v>
@@ -17672,7 +17686,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="95" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G20" s="95">
         <v>27.0</v>
@@ -17686,7 +17700,7 @@
         <v>141</v>
       </c>
       <c r="C21" s="89" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D21" s="90">
         <v>67.7</v>
@@ -17695,13 +17709,13 @@
         <v>1</v>
       </c>
       <c r="F21" s="85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G21" s="86">
         <v>32.3</v>
       </c>
       <c r="J21" s="93" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K21" s="94">
         <v>48.2</v>
@@ -17710,13 +17724,13 @@
         <v>1</v>
       </c>
       <c r="M21" s="85" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N21" s="86">
         <v>23.3</v>
       </c>
       <c r="O21" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P21" s="86">
         <v>16.7</v>
@@ -17730,7 +17744,7 @@
         <v>145</v>
       </c>
       <c r="J22" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K22" s="84">
         <v>35.9</v>
@@ -17739,13 +17753,13 @@
         <v>1</v>
       </c>
       <c r="M22" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N22" s="86">
         <v>31.6</v>
       </c>
       <c r="O22" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P22" s="86">
         <v>16.4</v>
@@ -17759,7 +17773,7 @@
         <v>150</v>
       </c>
       <c r="C23" s="87" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D23" s="88">
         <v>71.1</v>
@@ -17768,13 +17782,13 @@
         <v>1</v>
       </c>
       <c r="F23" s="85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G23" s="86">
         <v>23.2</v>
       </c>
       <c r="J23" s="83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K23" s="84">
         <v>41.4</v>
@@ -17783,13 +17797,13 @@
         <v>1</v>
       </c>
       <c r="M23" s="85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N23" s="86">
         <v>37.8</v>
       </c>
       <c r="O23" s="85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P23" s="86">
         <v>11.2</v>
@@ -17803,7 +17817,7 @@
         <v>153</v>
       </c>
       <c r="J24" s="93" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K24" s="94">
         <v>45.9</v>
@@ -17812,13 +17826,13 @@
         <v>1</v>
       </c>
       <c r="M24" s="85" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N24" s="86">
         <v>32.6</v>
       </c>
       <c r="O24" s="85" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="P24" s="86">
         <v>12.2</v>
@@ -17832,7 +17846,7 @@
         <v>156</v>
       </c>
       <c r="C25" s="89" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D25" s="90">
         <v>57.1</v>
@@ -17841,7 +17855,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G25" s="86">
         <v>42.9</v>
@@ -20800,13 +20814,13 @@
         <v>15</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>23</v>
@@ -20839,7 +20853,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
@@ -20855,14 +20869,14 @@
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="25" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="24"/>
       <c r="G3" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="4">
@@ -20874,14 +20888,14 @@
       </c>
       <c r="C4" s="25"/>
       <c r="D4" s="25" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E4" s="25" t="s">
         <v>33</v>
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5">
@@ -20892,7 +20906,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -20908,14 +20922,14 @@
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>43</v>
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7">
@@ -20927,14 +20941,14 @@
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="31" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>43</v>
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8">
@@ -20959,14 +20973,14 @@
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="25" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>53</v>
       </c>
       <c r="F9" s="24"/>
       <c r="G9" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10">
@@ -20978,14 +20992,14 @@
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="31" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>58</v>
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11">
@@ -21010,14 +21024,14 @@
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="25" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>53</v>
       </c>
       <c r="F12" s="24"/>
       <c r="G12" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="13">
@@ -21042,14 +21056,14 @@
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="31" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="24"/>
       <c r="G14" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="15">
@@ -21078,14 +21092,14 @@
       </c>
       <c r="C16" s="31"/>
       <c r="D16" s="31" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>70</v>
       </c>
       <c r="F16" s="24"/>
       <c r="G16" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17">
@@ -21097,14 +21111,14 @@
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="31" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>70</v>
       </c>
       <c r="F17" s="24"/>
       <c r="G17" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="18">
@@ -21116,14 +21130,14 @@
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="25" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>75</v>
       </c>
       <c r="F18" s="24"/>
       <c r="G18" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="19">
@@ -21135,14 +21149,14 @@
       </c>
       <c r="C19" s="48"/>
       <c r="D19" s="48" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E19" s="38" t="s">
         <v>131</v>
       </c>
       <c r="F19" s="37"/>
       <c r="G19" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="20">
@@ -21154,14 +21168,14 @@
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>79</v>
       </c>
       <c r="F20" s="24"/>
       <c r="G20" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="21">
@@ -21173,14 +21187,14 @@
       </c>
       <c r="C21" s="31"/>
       <c r="D21" s="31" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>79</v>
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="22">
@@ -21192,14 +21206,14 @@
       </c>
       <c r="C22" s="38"/>
       <c r="D22" s="38" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E22" s="38" t="s">
         <v>85</v>
       </c>
       <c r="F22" s="37"/>
       <c r="G22" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="23">
@@ -21211,14 +21225,14 @@
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="31" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>85</v>
       </c>
       <c r="F23" s="24"/>
       <c r="G23" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="24">
@@ -21230,14 +21244,14 @@
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="31" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F24" s="24"/>
       <c r="G24" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25">
@@ -21249,14 +21263,14 @@
       </c>
       <c r="C25" s="31"/>
       <c r="D25" s="31" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26">
@@ -21268,14 +21282,14 @@
       </c>
       <c r="C26" s="31"/>
       <c r="D26" s="31" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>97</v>
       </c>
       <c r="F26" s="24"/>
       <c r="G26" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="27">
@@ -21287,14 +21301,14 @@
       </c>
       <c r="C27" s="31"/>
       <c r="D27" s="31" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>97</v>
       </c>
       <c r="F27" s="24"/>
       <c r="G27" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="28">
@@ -21306,14 +21320,14 @@
       </c>
       <c r="C28" s="31"/>
       <c r="D28" s="31" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E28" s="25" t="s">
         <v>101</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="29">
@@ -21325,14 +21339,14 @@
       </c>
       <c r="C29" s="31"/>
       <c r="D29" s="31" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E29" s="25" t="s">
         <v>101</v>
       </c>
       <c r="F29" s="24"/>
       <c r="G29" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="30">
@@ -21344,14 +21358,14 @@
       </c>
       <c r="C30" s="38"/>
       <c r="D30" s="38" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F30" s="37"/>
       <c r="G30" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31">
@@ -21363,14 +21377,14 @@
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F31" s="24"/>
       <c r="G31" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="32">
@@ -21382,14 +21396,14 @@
       </c>
       <c r="C32" s="31"/>
       <c r="D32" s="31" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E32" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F32" s="24"/>
       <c r="G32" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="33">
@@ -21401,14 +21415,14 @@
       </c>
       <c r="C33" s="31"/>
       <c r="D33" s="31" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>109</v>
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="34">
@@ -21420,14 +21434,14 @@
       </c>
       <c r="C34" s="31"/>
       <c r="D34" s="31" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E34" s="25" t="s">
         <v>109</v>
       </c>
       <c r="F34" s="24"/>
       <c r="G34" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="35">
@@ -21439,14 +21453,14 @@
       </c>
       <c r="C35" s="31"/>
       <c r="D35" s="31" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E35" s="25" t="s">
         <v>113</v>
       </c>
       <c r="F35" s="24"/>
       <c r="G35" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="36">
@@ -21458,14 +21472,14 @@
       </c>
       <c r="C36" s="31"/>
       <c r="D36" s="31" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E36" s="25" t="s">
         <v>113</v>
       </c>
       <c r="F36" s="24"/>
       <c r="G36" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="37">
@@ -21477,14 +21491,14 @@
       </c>
       <c r="C37" s="31"/>
       <c r="D37" s="31" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>117</v>
       </c>
       <c r="F37" s="24"/>
       <c r="G37" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="38">
@@ -21496,14 +21510,14 @@
       </c>
       <c r="C38" s="31"/>
       <c r="D38" s="31" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>117</v>
       </c>
       <c r="F38" s="24"/>
       <c r="G38" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="39">
@@ -21515,14 +21529,14 @@
       </c>
       <c r="C39" s="31"/>
       <c r="D39" s="31" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>122</v>
       </c>
       <c r="F39" s="24"/>
       <c r="G39" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="40">
@@ -21534,14 +21548,14 @@
       </c>
       <c r="C40" s="31"/>
       <c r="D40" s="31" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E40" s="25" t="s">
         <v>122</v>
       </c>
       <c r="F40" s="24"/>
       <c r="G40" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="41">
@@ -21553,14 +21567,14 @@
       </c>
       <c r="C41" s="38"/>
       <c r="D41" s="38" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E41" s="38" t="s">
         <v>127</v>
       </c>
       <c r="F41" s="37"/>
       <c r="G41" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="42">
@@ -21568,7 +21582,7 @@
         <v>27</v>
       </c>
       <c r="B42" s="100" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21"/>
@@ -21585,14 +21599,14 @@
       </c>
       <c r="C43" s="31"/>
       <c r="D43" s="31" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E43" s="25" t="s">
         <v>142</v>
       </c>
       <c r="F43" s="24"/>
       <c r="G43" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="44">
@@ -21604,14 +21618,14 @@
       </c>
       <c r="C44" s="31"/>
       <c r="D44" s="31" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E44" s="25" t="s">
         <v>142</v>
       </c>
       <c r="F44" s="24"/>
       <c r="G44" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="45">
@@ -21623,14 +21637,14 @@
       </c>
       <c r="C45" s="31"/>
       <c r="D45" s="31" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E45" s="25" t="s">
         <v>146</v>
       </c>
       <c r="F45" s="101"/>
       <c r="G45" s="101" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="46">
@@ -21642,14 +21656,14 @@
       </c>
       <c r="C46" s="31"/>
       <c r="D46" s="31" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E46" s="25" t="s">
         <v>151</v>
       </c>
       <c r="F46" s="101"/>
       <c r="G46" s="101" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="47">
@@ -21661,14 +21675,14 @@
       </c>
       <c r="C47" s="31"/>
       <c r="D47" s="31" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E47" s="25" t="s">
         <v>151</v>
       </c>
       <c r="F47" s="101"/>
       <c r="G47" s="101" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="48">
@@ -21680,14 +21694,14 @@
       </c>
       <c r="C48" s="31"/>
       <c r="D48" s="31" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E48" s="25" t="s">
         <v>154</v>
       </c>
       <c r="F48" s="101"/>
       <c r="G48" s="101" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="49">
@@ -21699,14 +21713,14 @@
       </c>
       <c r="C49" s="31"/>
       <c r="D49" s="31" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E49" s="25" t="s">
         <v>157</v>
       </c>
       <c r="F49" s="24"/>
       <c r="G49" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="50">
@@ -21714,7 +21728,7 @@
         <v>27</v>
       </c>
       <c r="B50" s="100" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21"/>
@@ -21731,14 +21745,14 @@
       </c>
       <c r="C51" s="31"/>
       <c r="D51" s="31" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E51" s="25" t="s">
         <v>154</v>
       </c>
       <c r="F51" s="24"/>
       <c r="G51" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="52">
@@ -21750,14 +21764,14 @@
       </c>
       <c r="C52" s="31"/>
       <c r="D52" s="31" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E52" s="25" t="s">
         <v>163</v>
       </c>
       <c r="F52" s="24"/>
       <c r="G52" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="53">
@@ -21765,7 +21779,7 @@
         <v>27</v>
       </c>
       <c r="B53" s="100" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
@@ -21778,18 +21792,18 @@
         <v>15</v>
       </c>
       <c r="B54" s="98" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C54" s="31"/>
       <c r="D54" s="31" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F54" s="24"/>
       <c r="G54" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="55">
@@ -21797,18 +21811,18 @@
         <v>15</v>
       </c>
       <c r="B55" s="98" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C55" s="31"/>
       <c r="D55" s="31" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F55" s="24"/>
       <c r="G55" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="56">
@@ -21816,18 +21830,18 @@
         <v>15</v>
       </c>
       <c r="B56" s="99" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C56" s="38"/>
       <c r="D56" s="38" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E56" s="38" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F56" s="37"/>
       <c r="G56" s="37" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="57">
@@ -21835,18 +21849,18 @@
         <v>15</v>
       </c>
       <c r="B57" s="98" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C57" s="31"/>
       <c r="D57" s="31" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E57" s="25" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F57" s="24"/>
       <c r="G57" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="58">
@@ -21854,18 +21868,18 @@
         <v>15</v>
       </c>
       <c r="B58" s="98" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C58" s="31"/>
       <c r="D58" s="31" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E58" s="25" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F58" s="24"/>
       <c r="G58" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="59">
@@ -21873,18 +21887,18 @@
         <v>15</v>
       </c>
       <c r="B59" s="98" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C59" s="31"/>
       <c r="D59" s="31" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E59" s="25" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F59" s="24"/>
       <c r="G59" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="60">
@@ -21892,18 +21906,18 @@
         <v>15</v>
       </c>
       <c r="B60" s="98" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C60" s="31"/>
       <c r="D60" s="31" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E60" s="25" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F60" s="24"/>
       <c r="G60" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="61">
@@ -21911,7 +21925,7 @@
         <v>27</v>
       </c>
       <c r="B61" s="100" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C61" s="21"/>
       <c r="D61" s="21"/>
@@ -21924,18 +21938,18 @@
         <v>15</v>
       </c>
       <c r="B62" s="98" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C62" s="25"/>
       <c r="D62" s="25" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E62" s="25" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F62" s="24"/>
       <c r="G62" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="63">
@@ -21943,18 +21957,18 @@
         <v>15</v>
       </c>
       <c r="B63" s="99" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C63" s="38"/>
       <c r="D63" s="38" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E63" s="38" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F63" s="37"/>
       <c r="G63" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="64">
@@ -21962,18 +21976,18 @@
         <v>15</v>
       </c>
       <c r="B64" s="98" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C64" s="31"/>
       <c r="D64" s="31" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E64" s="25" t="s">
         <v>127</v>
       </c>
       <c r="F64" s="24"/>
       <c r="G64" s="24" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="65">
@@ -21981,10 +21995,10 @@
         <v>27</v>
       </c>
       <c r="B65" s="100" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D65" s="17"/>
       <c r="E65" s="17"/>
@@ -21996,18 +22010,18 @@
         <v>15</v>
       </c>
       <c r="B66" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C66" s="31"/>
       <c r="D66" s="31" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E66" s="25" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F66" s="24"/>
       <c r="G66" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="67">
@@ -22015,18 +22029,18 @@
         <v>15</v>
       </c>
       <c r="B67" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C67" s="31"/>
       <c r="D67" s="31" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E67" s="25" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F67" s="24"/>
       <c r="G67" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="68">
@@ -22034,18 +22048,18 @@
         <v>15</v>
       </c>
       <c r="B68" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C68" s="31"/>
       <c r="D68" s="31" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E68" s="25" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F68" s="24"/>
       <c r="G68" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="69">
@@ -22053,18 +22067,18 @@
         <v>15</v>
       </c>
       <c r="B69" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C69" s="31"/>
       <c r="D69" s="31" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E69" s="25" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F69" s="24"/>
       <c r="G69" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="70">
@@ -22072,18 +22086,18 @@
         <v>15</v>
       </c>
       <c r="B70" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C70" s="31"/>
       <c r="D70" s="31" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E70" s="25" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F70" s="24"/>
       <c r="G70" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="71">
@@ -22091,18 +22105,18 @@
         <v>15</v>
       </c>
       <c r="B71" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="31" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E71" s="25" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F71" s="24"/>
       <c r="G71" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="72">
@@ -22110,18 +22124,18 @@
         <v>15</v>
       </c>
       <c r="B72" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C72" s="31"/>
       <c r="D72" s="31" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E72" s="25" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F72" s="24"/>
       <c r="G72" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="73">
@@ -22129,18 +22143,18 @@
         <v>15</v>
       </c>
       <c r="B73" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C73" s="31"/>
       <c r="D73" s="31" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E73" s="25" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F73" s="24"/>
       <c r="G73" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="74">
@@ -22148,18 +22162,18 @@
         <v>15</v>
       </c>
       <c r="B74" s="99" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C74" s="38"/>
       <c r="D74" s="38" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E74" s="38" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F74" s="37"/>
       <c r="G74" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="75">
@@ -22167,18 +22181,18 @@
         <v>15</v>
       </c>
       <c r="B75" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C75" s="31"/>
       <c r="D75" s="31" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E75" s="25" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F75" s="24"/>
       <c r="G75" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="76">
@@ -22186,18 +22200,18 @@
         <v>15</v>
       </c>
       <c r="B76" s="98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C76" s="31"/>
       <c r="D76" s="31" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E76" s="25" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F76" s="24"/>
       <c r="G76" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="77">
@@ -22205,7 +22219,7 @@
         <v>27</v>
       </c>
       <c r="B77" s="100" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C77" s="21"/>
       <c r="D77" s="21"/>
@@ -22218,18 +22232,18 @@
         <v>15</v>
       </c>
       <c r="B78" s="99" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C78" s="38"/>
       <c r="D78" s="38" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E78" s="38" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F78" s="37"/>
       <c r="G78" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="79">
@@ -22237,7 +22251,7 @@
         <v>27</v>
       </c>
       <c r="B79" s="100" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C79" s="21"/>
       <c r="D79" s="21"/>
@@ -22250,18 +22264,18 @@
         <v>15</v>
       </c>
       <c r="B80" s="99" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C80" s="38"/>
       <c r="D80" s="38" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E80" s="38" t="s">
         <v>131</v>
       </c>
       <c r="F80" s="37"/>
       <c r="G80" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="81">
@@ -22269,18 +22283,18 @@
         <v>15</v>
       </c>
       <c r="B81" s="98" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C81" s="31"/>
       <c r="D81" s="31" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E81" s="25" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F81" s="24"/>
       <c r="G81" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="82">
@@ -22288,18 +22302,18 @@
         <v>15</v>
       </c>
       <c r="B82" s="98" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C82" s="31"/>
       <c r="D82" s="31" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E82" s="25" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F82" s="24"/>
       <c r="G82" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="83">
@@ -22307,18 +22321,18 @@
         <v>15</v>
       </c>
       <c r="B83" s="98" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C83" s="25"/>
       <c r="D83" s="25" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="E83" s="25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F83" s="24"/>
       <c r="G83" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="84">
@@ -22326,18 +22340,18 @@
         <v>15</v>
       </c>
       <c r="B84" s="98" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C84" s="25"/>
       <c r="D84" s="25" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E84" s="25" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F84" s="24"/>
       <c r="G84" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="85">
@@ -22345,16 +22359,16 @@
         <v>15</v>
       </c>
       <c r="B85" s="98" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C85" s="25"/>
       <c r="D85" s="25" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E85" s="31"/>
       <c r="F85" s="24"/>
       <c r="G85" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="86">
@@ -22362,7 +22376,7 @@
         <v>27</v>
       </c>
       <c r="B86" s="100" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C86" s="21"/>
       <c r="D86" s="21"/>
@@ -22375,18 +22389,18 @@
         <v>15</v>
       </c>
       <c r="B87" s="98" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C87" s="25"/>
       <c r="D87" s="25" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E87" s="25" t="s">
         <v>75</v>
       </c>
       <c r="F87" s="24"/>
       <c r="G87" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="88">
@@ -22394,18 +22408,18 @@
         <v>15</v>
       </c>
       <c r="B88" s="98" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C88" s="25"/>
       <c r="D88" s="25" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E88" s="25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F88" s="24"/>
       <c r="G88" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="89">
@@ -22413,18 +22427,18 @@
         <v>15</v>
       </c>
       <c r="B89" s="98" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C89" s="31"/>
       <c r="D89" s="31" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E89" s="25" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F89" s="24"/>
       <c r="G89" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="90">
@@ -22432,7 +22446,7 @@
         <v>27</v>
       </c>
       <c r="B90" s="100" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C90" s="21"/>
       <c r="D90" s="21"/>
@@ -22445,18 +22459,18 @@
         <v>15</v>
       </c>
       <c r="B91" s="98" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C91" s="31"/>
       <c r="D91" s="31" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E91" s="25" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F91" s="24"/>
       <c r="G91" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="92">
@@ -22464,18 +22478,18 @@
         <v>15</v>
       </c>
       <c r="B92" s="98" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C92" s="31"/>
       <c r="D92" s="31" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E92" s="25" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F92" s="24"/>
       <c r="G92" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="93">
@@ -22483,7 +22497,7 @@
         <v>27</v>
       </c>
       <c r="B93" s="100" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C93" s="21"/>
       <c r="D93" s="21"/>
@@ -22496,18 +22510,18 @@
         <v>15</v>
       </c>
       <c r="B94" s="98" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C94" s="25"/>
       <c r="D94" s="25" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E94" s="25" t="s">
         <v>127</v>
       </c>
       <c r="F94" s="24"/>
       <c r="G94" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="95">
@@ -22515,7 +22529,7 @@
         <v>27</v>
       </c>
       <c r="B95" s="100" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C95" s="21"/>
       <c r="D95" s="21"/>
@@ -22528,18 +22542,18 @@
         <v>15</v>
       </c>
       <c r="B96" s="98" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C96" s="31"/>
       <c r="D96" s="31" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E96" s="25" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F96" s="24"/>
       <c r="G96" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="97">
@@ -22547,18 +22561,18 @@
         <v>15</v>
       </c>
       <c r="B97" s="98" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C97" s="31"/>
       <c r="D97" s="31" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E97" s="25" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F97" s="24"/>
       <c r="G97" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="98">
@@ -22566,7 +22580,7 @@
         <v>27</v>
       </c>
       <c r="B98" s="100" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C98" s="21"/>
       <c r="D98" s="21"/>
@@ -22579,18 +22593,18 @@
         <v>15</v>
       </c>
       <c r="B99" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C99" s="31"/>
       <c r="D99" s="31" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E99" s="25" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F99" s="24"/>
       <c r="G99" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="100">
@@ -22598,18 +22612,18 @@
         <v>15</v>
       </c>
       <c r="B100" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C100" s="31"/>
       <c r="D100" s="31" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E100" s="25" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F100" s="24"/>
       <c r="G100" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="101">
@@ -22617,18 +22631,18 @@
         <v>15</v>
       </c>
       <c r="B101" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C101" s="31"/>
       <c r="D101" s="31" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E101" s="25" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F101" s="24"/>
       <c r="G101" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="102">
@@ -22636,18 +22650,18 @@
         <v>15</v>
       </c>
       <c r="B102" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C102" s="31"/>
       <c r="D102" s="31" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E102" s="25" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F102" s="24"/>
       <c r="G102" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="103">
@@ -22655,18 +22669,18 @@
         <v>15</v>
       </c>
       <c r="B103" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C103" s="31"/>
       <c r="D103" s="31" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E103" s="25" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F103" s="24"/>
       <c r="G103" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="104">
@@ -22674,18 +22688,18 @@
         <v>15</v>
       </c>
       <c r="B104" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C104" s="31"/>
       <c r="D104" s="31" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E104" s="25" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F104" s="24"/>
       <c r="G104" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="105">
@@ -22693,18 +22707,18 @@
         <v>15</v>
       </c>
       <c r="B105" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C105" s="31"/>
       <c r="D105" s="31" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E105" s="25" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F105" s="24"/>
       <c r="G105" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="106">
@@ -22712,18 +22726,18 @@
         <v>15</v>
       </c>
       <c r="B106" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C106" s="31"/>
       <c r="D106" s="31" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E106" s="25" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F106" s="24"/>
       <c r="G106" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="107">
@@ -22731,18 +22745,18 @@
         <v>15</v>
       </c>
       <c r="B107" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C107" s="31"/>
       <c r="D107" s="31" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E107" s="25" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F107" s="24"/>
       <c r="G107" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="108">
@@ -22750,18 +22764,18 @@
         <v>15</v>
       </c>
       <c r="B108" s="98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C108" s="31"/>
       <c r="D108" s="31" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="E108" s="25" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F108" s="24"/>
       <c r="G108" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="109">
@@ -22769,7 +22783,7 @@
         <v>27</v>
       </c>
       <c r="B109" s="100" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C109" s="21"/>
       <c r="D109" s="21"/>
@@ -22782,18 +22796,18 @@
         <v>15</v>
       </c>
       <c r="B110" s="98" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C110" s="31"/>
       <c r="D110" s="31" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E110" s="25" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F110" s="24"/>
       <c r="G110" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="111">
@@ -22801,18 +22815,18 @@
         <v>15</v>
       </c>
       <c r="B111" s="98" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C111" s="31"/>
       <c r="D111" s="31" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E111" s="25" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F111" s="24"/>
       <c r="G111" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="112">
@@ -22820,7 +22834,7 @@
         <v>27</v>
       </c>
       <c r="B112" s="100" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C112" s="21"/>
       <c r="D112" s="21"/>
@@ -22833,18 +22847,18 @@
         <v>15</v>
       </c>
       <c r="B113" s="99" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C113" s="38"/>
       <c r="D113" s="38" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E113" s="38" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F113" s="37"/>
       <c r="G113" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="114">
@@ -22852,7 +22866,7 @@
         <v>27</v>
       </c>
       <c r="B114" s="100" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C114" s="21"/>
       <c r="D114" s="21"/>
@@ -22865,18 +22879,18 @@
         <v>15</v>
       </c>
       <c r="B115" s="98" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C115" s="31"/>
       <c r="D115" s="31" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="E115" s="25" t="s">
         <v>157</v>
       </c>
       <c r="F115" s="24"/>
       <c r="G115" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="116">
@@ -22884,18 +22898,18 @@
         <v>15</v>
       </c>
       <c r="B116" s="98" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C116" s="25"/>
       <c r="D116" s="25" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E116" s="25" t="s">
         <v>157</v>
       </c>
       <c r="F116" s="24"/>
       <c r="G116" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="117">
@@ -22903,18 +22917,18 @@
         <v>15</v>
       </c>
       <c r="B117" s="98" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C117" s="31"/>
       <c r="D117" s="31" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="E117" s="25" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F117" s="24"/>
       <c r="G117" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="118">
@@ -22922,18 +22936,18 @@
         <v>15</v>
       </c>
       <c r="B118" s="98" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C118" s="31"/>
       <c r="D118" s="31" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E118" s="25" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F118" s="24"/>
       <c r="G118" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="119">
@@ -22941,7 +22955,7 @@
         <v>27</v>
       </c>
       <c r="B119" s="100" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C119" s="21"/>
       <c r="D119" s="21"/>
@@ -22954,18 +22968,18 @@
         <v>15</v>
       </c>
       <c r="B120" s="98" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C120" s="31"/>
       <c r="D120" s="31" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E120" s="25" t="s">
         <v>146</v>
       </c>
       <c r="F120" s="24"/>
       <c r="G120" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="121">
@@ -22973,18 +22987,18 @@
         <v>15</v>
       </c>
       <c r="B121" s="98" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C121" s="31"/>
       <c r="D121" s="31" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="E121" s="25" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F121" s="24"/>
       <c r="G121" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="122">
@@ -22992,18 +23006,18 @@
         <v>15</v>
       </c>
       <c r="B122" s="98" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C122" s="31"/>
       <c r="D122" s="31" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="E122" s="25" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F122" s="24"/>
       <c r="G122" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="123">
@@ -23011,7 +23025,7 @@
         <v>27</v>
       </c>
       <c r="B123" s="100" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C123" s="21"/>
       <c r="D123" s="21"/>
@@ -23024,18 +23038,18 @@
         <v>15</v>
       </c>
       <c r="B124" s="98" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C124" s="25"/>
       <c r="D124" s="25" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E124" s="25" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F124" s="24"/>
       <c r="G124" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="125">
@@ -23043,18 +23057,18 @@
         <v>15</v>
       </c>
       <c r="B125" s="98" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C125" s="31"/>
       <c r="D125" s="31" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E125" s="25" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F125" s="24"/>
       <c r="G125" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="126">
@@ -23062,7 +23076,7 @@
         <v>27</v>
       </c>
       <c r="B126" s="100" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C126" s="21"/>
       <c r="D126" s="21"/>
@@ -23075,18 +23089,18 @@
         <v>15</v>
       </c>
       <c r="B127" s="99" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C127" s="48"/>
       <c r="D127" s="48" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E127" s="38" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F127" s="37"/>
       <c r="G127" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="128">
@@ -23094,7 +23108,7 @@
         <v>27</v>
       </c>
       <c r="B128" s="102" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C128" s="21"/>
       <c r="D128" s="21"/>
@@ -23107,18 +23121,18 @@
         <v>15</v>
       </c>
       <c r="B129" s="103" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C129" s="63"/>
       <c r="D129" s="63" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E129" s="64" t="s">
         <v>163</v>
       </c>
       <c r="F129" s="62"/>
       <c r="G129" s="62" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="130">
@@ -23126,7 +23140,7 @@
         <v>27</v>
       </c>
       <c r="B130" s="100" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C130" s="21"/>
       <c r="D130" s="21"/>
@@ -23139,18 +23153,18 @@
         <v>15</v>
       </c>
       <c r="B131" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C131" s="31"/>
       <c r="D131" s="31" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E131" s="25" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F131" s="24"/>
       <c r="G131" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="132">
@@ -23158,18 +23172,18 @@
         <v>15</v>
       </c>
       <c r="B132" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C132" s="31"/>
       <c r="D132" s="31" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="E132" s="25" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F132" s="24"/>
       <c r="G132" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="133">
@@ -23177,18 +23191,18 @@
         <v>15</v>
       </c>
       <c r="B133" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C133" s="31"/>
       <c r="D133" s="31" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E133" s="25" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F133" s="24"/>
       <c r="G133" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="134">
@@ -23196,18 +23210,18 @@
         <v>15</v>
       </c>
       <c r="B134" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C134" s="31"/>
       <c r="D134" s="31" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E134" s="25" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F134" s="24"/>
       <c r="G134" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="135">
@@ -23215,18 +23229,18 @@
         <v>15</v>
       </c>
       <c r="B135" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C135" s="31"/>
       <c r="D135" s="31" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E135" s="25" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F135" s="24"/>
       <c r="G135" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="136">
@@ -23234,18 +23248,18 @@
         <v>15</v>
       </c>
       <c r="B136" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C136" s="31"/>
       <c r="D136" s="31" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E136" s="25" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F136" s="24"/>
       <c r="G136" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="137">
@@ -23253,18 +23267,18 @@
         <v>15</v>
       </c>
       <c r="B137" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C137" s="31"/>
       <c r="D137" s="31" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="E137" s="25" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F137" s="24"/>
       <c r="G137" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="138">
@@ -23272,18 +23286,18 @@
         <v>15</v>
       </c>
       <c r="B138" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C138" s="31"/>
       <c r="D138" s="31" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E138" s="25" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F138" s="24"/>
       <c r="G138" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="139">
@@ -23291,18 +23305,18 @@
         <v>15</v>
       </c>
       <c r="B139" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C139" s="31"/>
       <c r="D139" s="31" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E139" s="25" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F139" s="24"/>
       <c r="G139" s="24" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="140">
@@ -23310,18 +23324,18 @@
         <v>15</v>
       </c>
       <c r="B140" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C140" s="31"/>
       <c r="D140" s="31" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E140" s="25" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F140" s="24"/>
       <c r="G140" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="141">
@@ -23329,18 +23343,18 @@
         <v>15</v>
       </c>
       <c r="B141" s="98" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C141" s="31"/>
       <c r="D141" s="31" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E141" s="25" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F141" s="24"/>
       <c r="G141" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="142">
@@ -23348,7 +23362,7 @@
         <v>27</v>
       </c>
       <c r="B142" s="100" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C142" s="21"/>
       <c r="D142" s="21"/>
@@ -23361,18 +23375,18 @@
         <v>15</v>
       </c>
       <c r="B143" s="98" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C143" s="31"/>
       <c r="D143" s="31" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E143" s="25" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F143" s="24"/>
       <c r="G143" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="144">

</xml_diff>

<commit_message>
feed new live audio card from gdoc
</commit_message>
<xml_diff>
--- a/data/calendar.xlsx
+++ b/data/calendar.xlsx
@@ -632,13 +632,13 @@
     <t>Convention</t>
   </si>
   <si>
-    <t>Polls close at 7 pm</t>
+    <t>Caucusing ends at 4:00 p.m. EST</t>
   </si>
   <si>
     <t>Republican county conventions&lt;sup&gt;2&lt;/sup&gt;</t>
   </si>
   <si>
-    <t>Polls close at 8 pm</t>
+    <t>Caucusing begins at 10 a.m. EST</t>
   </si>
   <si>
     <t>Guam</t>
@@ -4027,7 +4027,7 @@
         <v>204</v>
       </c>
       <c r="O46" s="34" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47">
@@ -4061,7 +4061,7 @@
         <v>206</v>
       </c>
       <c r="O47" s="34" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48">

</xml_diff>